<commit_message>
update MOQA code and reports
</commit_message>
<xml_diff>
--- a/Data quality revision R overview v01.xlsx
+++ b/Data quality revision R overview v01.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="420">
   <si>
     <t>Acronym (falls vorhanden)</t>
   </si>
@@ -506,12 +506,6 @@
     <t>R objects (JSON for validatereport)</t>
   </si>
   <si>
-    <t>yes, as "validation rules" (text and yaml files)</t>
-  </si>
-  <si>
-    <t>yes, as "validation rules"</t>
-  </si>
-  <si>
     <t>Field length (number of characters in text fields)</t>
   </si>
   <si>
@@ -545,9 +539,6 @@
     <t>Forbidden value combinations</t>
   </si>
   <si>
-    <t>handling long format data, comparing data sets (with lumberjack package), statistical checks, continuous data indicators</t>
-  </si>
-  <si>
     <t>yes, iff using validatereport package (in beta version only - does not work)</t>
   </si>
   <si>
@@ -630,9 +621,6 @@
   </si>
   <si>
     <t>Quantify missing values</t>
-  </si>
-  <si>
-    <t>outliers</t>
   </si>
   <si>
     <t>dataClean</t>
@@ -1318,6 +1306,39 @@
   </si>
   <si>
     <t>Variable type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean, min, med, max, quartiles, outliers, </t>
+  </si>
+  <si>
+    <t>Types</t>
+  </si>
+  <si>
+    <t>handling long format data, comparing data sets (with lumberjack package), statistical checks, continuous data indicators. Integration with Statistical Data and Metadata eXchange (SDMX) and Data Structure Definition (DSD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, as "validation rules" or from SDMX or DSD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, as "validation rules" (text and yaml files) or from SDMX or DSD </t>
+  </si>
+  <si>
+    <t>yes, for the "validation rules"</t>
+  </si>
+  <si>
+    <t>yes (one report per variable)</t>
+  </si>
+  <si>
+    <t>Missings (but it doesn't seem to work)</t>
+  </si>
+  <si>
+    <t>Empirical distribution</t>
+  </si>
+  <si>
+    <t>Outliers (from box-whisker plot)</t>
+  </si>
+  <si>
+    <t>Frequency, percentage, empirical distribution, mean, min, max, quartiles, box-whisker plot, qq-plot</t>
   </si>
 </sst>
 </file>
@@ -1727,11 +1748,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="S27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="T43" sqref="T43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1796,118 +1817,118 @@
         <v>66</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="T1" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>187</v>
-      </c>
       <c r="W1" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="AA1" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="AD1" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>329</v>
-      </c>
       <c r="AH1" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="AL1" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="AR1" s="4" t="s">
-        <v>393</v>
-      </c>
-      <c r="AS1" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="AT1" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="AU1" s="4" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="2" spans="1:47" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -1930,61 +1951,61 @@
         <v>71</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>149</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="O2" s="2" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.25">
@@ -2067,7 +2088,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:47" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -2090,61 +2111,61 @@
         <v>144</v>
       </c>
       <c r="H4" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="I4" t="s">
         <v>50</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="K4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>53</v>
       </c>
       <c r="M4" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="N4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="O4" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="P4" t="s">
         <v>144</v>
       </c>
       <c r="Q4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="R4" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="S4" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="T4" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="U4" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="V4" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="W4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="X4" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="Y4" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="Z4" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="5" spans="1:47" ht="30" x14ac:dyDescent="0.25">
@@ -2268,7 +2289,7 @@
         <v>19</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>19</v>
@@ -2333,10 +2354,10 @@
         <v>13</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>13</v>
+        <v>415</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>19</v>
@@ -2481,7 +2502,7 @@
         <v>130</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>68</v>
@@ -2490,61 +2511,61 @@
         <v>76</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>156</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="R9" s="7" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="S9" s="7" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="U9" s="7" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="V9" s="7" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="W9" s="7" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="X9" s="7" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="Y9" s="7" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="Z9" s="7" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="10" spans="1:47" ht="30" x14ac:dyDescent="0.25">
@@ -2656,7 +2677,7 @@
         <v>53</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>15</v>
@@ -2665,7 +2686,7 @@
         <v>15</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>15</v>
@@ -2736,7 +2757,7 @@
         <v>53</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>15</v>
@@ -2745,7 +2766,7 @@
         <v>15</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>15</v>
@@ -3028,7 +3049,7 @@
         <v>14</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>133</v>
@@ -3040,46 +3061,46 @@
         <v>147</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>173</v>
+        <v>411</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="P17" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q17" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="Q17" s="2" t="s">
-        <v>276</v>
-      </c>
       <c r="S17" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="18" spans="1:26" ht="30" x14ac:dyDescent="0.25">
@@ -3105,7 +3126,7 @@
         <v>19</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>161</v>
+        <v>412</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>19</v>
@@ -3120,22 +3141,22 @@
         <v>19</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="Q18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="T18" s="2" t="s">
         <v>19</v>
@@ -3182,7 +3203,7 @@
         <v>19</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>160</v>
+        <v>413</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>19</v>
@@ -3197,22 +3218,22 @@
         <v>19</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="Q19" s="2" t="s">
         <v>19</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="T19" s="2" t="s">
         <v>19</v>
@@ -3259,7 +3280,7 @@
         <v>19</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>13</v>
+        <v>414</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>19</v>
@@ -3313,7 +3334,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
@@ -3336,61 +3357,61 @@
         <v>75</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>159</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="M21" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="N21" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="N21" s="2" t="s">
-        <v>244</v>
-      </c>
       <c r="O21" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="W21" s="2" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="X21" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="Y21" s="2" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="Z21" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="22" spans="1:26" ht="30" x14ac:dyDescent="0.25">
@@ -3470,7 +3491,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>37</v>
       </c>
@@ -3508,7 +3529,7 @@
         <v>19</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="O23" s="2" t="s">
         <v>19</v>
@@ -3646,37 +3667,37 @@
         <v>153</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="T25" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="V25" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="Y25" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="Z25" s="3" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="26" spans="1:26" ht="45" x14ac:dyDescent="0.25">
@@ -3702,55 +3723,55 @@
         <v>143</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="I26" s="3" t="s">
         <v>150</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="K26" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="L26" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="L26" s="3" t="s">
-        <v>211</v>
-      </c>
       <c r="M26" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="Q26" s="3" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="R26" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="S26" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="S26" s="3" t="s">
-        <v>287</v>
-      </c>
       <c r="T26" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="U26" s="3" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="V26" s="3" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="X26" s="3" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="Z26" s="3" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="27" spans="1:26" ht="60" x14ac:dyDescent="0.25">
@@ -3776,37 +3797,37 @@
         <v>72</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="I27" s="12" t="s">
         <v>154</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="Q27" s="3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="T27" s="3" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="U27" s="3" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="V27" s="3" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="W27" s="3" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="X27" s="3" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="Y27" s="3" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="28" spans="1:26" ht="45" x14ac:dyDescent="0.25">
@@ -3832,55 +3853,55 @@
         <v>72</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>155</v>
       </c>
       <c r="J28" s="12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="N28" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="Q28" s="3" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="R28" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="S28" s="3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="T28" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="U28" s="3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="V28" s="3" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="W28" s="3" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="Y28" s="3" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="Z28" s="3" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="29" spans="1:26" ht="45" x14ac:dyDescent="0.25">
@@ -3896,16 +3917,16 @@
         <v>158</v>
       </c>
       <c r="W29" s="3" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="Z29" s="3" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>33</v>
       </c>
@@ -3934,19 +3955,19 @@
         <v>151</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>151</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>151</v>
       </c>
       <c r="N31" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="O31" s="2" t="s">
         <v>151</v>
@@ -3964,16 +3985,16 @@
         <v>151</v>
       </c>
       <c r="T31" s="5" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="U31" s="5" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="V31" s="5" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="W31" s="5" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="X31" s="2" t="s">
         <v>151</v>
@@ -3985,7 +4006,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>78</v>
       </c>
@@ -4065,7 +4086,7 @@
         <v>41058</v>
       </c>
     </row>
-    <row r="33" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>118</v>
       </c>
@@ -4168,13 +4189,13 @@
         <v>73</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>152</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>119</v>
@@ -4183,34 +4204,34 @@
         <v>119</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="P34" s="2" t="s">
         <v>119</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="T34" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="U34" s="5" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="V34" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="W34" s="2">
         <v>1.2</v>
@@ -4219,87 +4240,93 @@
         <v>0.1</v>
       </c>
       <c r="Y34" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="Z34" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="36" spans="1:26" ht="117.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>410</v>
+        <v>406</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>419</v>
       </c>
       <c r="U36" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="V36" s="2" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="Y36" s="2" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="37" spans="1:26" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="E37" s="6"/>
       <c r="H37" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="V37" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="W37" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="X37" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="Y37" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.25">
@@ -4323,7 +4350,7 @@
         <v>79</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.25">
@@ -4334,13 +4361,10 @@
         <v>80</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>168</v>
+        <v>403</v>
       </c>
       <c r="Z43" s="2" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.25">
@@ -4357,10 +4381,10 @@
         <v>81</v>
       </c>
       <c r="T44" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="Z44" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.25">
@@ -4371,7 +4395,7 @@
         <v>82</v>
       </c>
       <c r="Z45" s="2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.25">
@@ -4393,16 +4417,19 @@
         <v>127</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>412</v>
+        <v>408</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>410</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>157</v>
       </c>
       <c r="Y47" s="2" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="Z47" s="2" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="48" spans="1:26" ht="30" x14ac:dyDescent="0.25">
@@ -4416,7 +4443,7 @@
         <v>124</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="49" spans="1:26" ht="30" x14ac:dyDescent="0.25">
@@ -4439,22 +4466,25 @@
         <v>145</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>416</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="U49" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="V49" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="Y49" s="2" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="Z49" s="2" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.25">
@@ -4462,27 +4492,27 @@
         <v>126</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="L50" s="2" t="s">
         <v>126</v>
       </c>
       <c r="V50" s="2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="51" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="D51" s="2" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="52" spans="1:26" ht="30" x14ac:dyDescent="0.25">
@@ -4490,10 +4520,15 @@
         <v>129</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="Y52" s="2" t="s">
-        <v>400</v>
+        <v>396</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="I53" s="2" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.25">
@@ -4508,9 +4543,6 @@
       <c r="C55" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="J55" s="2" t="s">
-        <v>201</v>
-      </c>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
@@ -4544,10 +4576,10 @@
         <v>93</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.25">
@@ -4557,13 +4589,13 @@
     </row>
     <row r="62" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>95</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.25">
@@ -4574,7 +4606,7 @@
         <v>96</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="64" spans="1:26" ht="30" x14ac:dyDescent="0.25">
@@ -4585,7 +4617,7 @@
         <v>97</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="65" spans="1:22" ht="30" x14ac:dyDescent="0.25">
@@ -4606,13 +4638,13 @@
     </row>
     <row r="67" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>100</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.25">
@@ -4623,7 +4655,7 @@
         <v>101</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" spans="1:22" ht="30" x14ac:dyDescent="0.25">
@@ -4634,7 +4666,7 @@
         <v>102</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.25">
@@ -4647,7 +4679,7 @@
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="I71" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.25">
@@ -4669,10 +4701,10 @@
         <v>146</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>202</v>
+        <v>418</v>
       </c>
       <c r="V74" s="2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.25">
@@ -4698,8 +4730,14 @@
       <c r="C77" s="2" t="s">
         <v>108</v>
       </c>
+      <c r="D77" s="2" t="s">
+        <v>407</v>
+      </c>
       <c r="E77" s="2" t="s">
-        <v>411</v>
+        <v>407</v>
+      </c>
+      <c r="J77" s="2" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.25">
@@ -4726,7 +4764,7 @@
         <v>111</v>
       </c>
       <c r="U80" s="2" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="81" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4737,7 +4775,7 @@
         <v>112</v>
       </c>
       <c r="U81" s="2" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add explore code and report
</commit_message>
<xml_diff>
--- a/Data quality revision R overview v01.xlsx
+++ b/Data quality revision R overview v01.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="469">
   <si>
     <t>Acronym (falls vorhanden)</t>
   </si>
@@ -1302,9 +1302,6 @@
     <t>Variable type</t>
   </si>
   <si>
-    <t xml:space="preserve">mean, min, med, max, quartiles, outliers, </t>
-  </si>
-  <si>
     <t>Types</t>
   </si>
   <si>
@@ -1414,6 +1411,82 @@
   </si>
   <si>
     <t xml:space="preserve">Automated exploratory data analysis for modelling problems, variables of interest and data of interest. Exploratory data analysis can be performed both visually and in a tabular manner. In addition allows for exploring variable predictive power when encountering a modelling problem. autoEDA aims to automate exploratory data analysis in a univariate or bivariate manner. It has the ability to output plots created with the ggplot2 library and themes inspired by RColorBrewer. The main ability involves seemlessly cleaning and pre-processing your data inorder for plots to display adequately. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExPanDaR </t>
+  </si>
+  <si>
+    <t>0.5.3</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=ExPanDaR</t>
+  </si>
+  <si>
+    <t>https://joachim-gassen.github.io/ExPanDaR/</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Extreme observations</t>
+  </si>
+  <si>
+    <t>Correlation plot</t>
+  </si>
+  <si>
+    <t>mean, median, sd, min, max, quartiles, histogram. Bar, violin, scatter plots by group. Regression analysis.</t>
+  </si>
+  <si>
+    <t>https://github.com/joachim-gassen/ExPanDaR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExPanD has two purposes: 1) Provide a toolbox for researchers to explore data on the fly, now also allowing them to download R notebook code that reflects their analysis. 2) Enable users to assess the robustness of empirical evidence without providing them with access to the underlying data. Provides a shiny-based front end (the 'ExPanD' app) and a set of functions for exploratory data analysis. Run as a web-based app, 'ExPanD' enables users to assess the robustness of empirical evidence without providing them access to the underlying data. You can export a notebook containing the analysis of 'ExPanD' and/or use the functions of the package to support your exploratory data analysis workflow.
+</t>
+  </si>
+  <si>
+    <t>yes, as "df_def"</t>
+  </si>
+  <si>
+    <t>R objects, Rmd, html</t>
+  </si>
+  <si>
+    <t>explore</t>
+  </si>
+  <si>
+    <t>Interactive data exploration with one line of code or use an easy to remember set of tidy functions for exploratory data analysis. Introduces three main verbs. explore() to graphically explore a variable or table, describe() to describe a variable or table and report() to create an automated report.</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>min, mean, max, boxplots</t>
+  </si>
+  <si>
+    <t>Decision tree and logistic regression</t>
+  </si>
+  <si>
+    <t>https://github.com/rolkra/explore</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=explore</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/web/packages/explore/vignettes/explore.html</t>
+  </si>
+  <si>
+    <t>0.7.1</t>
+  </si>
+  <si>
+    <t>explore_cor</t>
+  </si>
+  <si>
+    <t>Correlation coefficient, matrix and plot</t>
+  </si>
+  <si>
+    <t>mean, min, med, max, quartiles, outliers, normality test</t>
   </si>
 </sst>
 </file>
@@ -1821,286 +1894,292 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU85"/>
+  <dimension ref="A1:AV85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AB3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="X32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AB9" sqref="AB9"/>
+      <selection pane="bottomRight" activeCell="X36" sqref="X36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="47" style="2" customWidth="1"/>
-    <col min="4" max="4" width="43.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="46.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="39.5703125" style="2" customWidth="1"/>
-    <col min="7" max="8" width="38.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="42" style="2" customWidth="1"/>
-    <col min="10" max="10" width="40.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="32.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="33.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="34.28515625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="38.7109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="32.5703125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="31.7109375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="32.7109375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="36.42578125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="33.28515625" style="2" customWidth="1"/>
-    <col min="20" max="20" width="34" style="2" customWidth="1"/>
-    <col min="21" max="21" width="33.28515625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="38.7109375" style="2" customWidth="1"/>
-    <col min="23" max="23" width="34.42578125" style="2" customWidth="1"/>
-    <col min="24" max="24" width="33" style="2" customWidth="1"/>
-    <col min="25" max="25" width="33.85546875" style="2" customWidth="1"/>
-    <col min="26" max="26" width="32.85546875" style="2" customWidth="1"/>
-    <col min="27" max="27" width="36.42578125" style="2" customWidth="1"/>
-    <col min="28" max="28" width="32.7109375" style="2" customWidth="1"/>
-    <col min="29" max="16384" width="11" style="2"/>
+    <col min="1" max="1" width="11" style="2"/>
+    <col min="2" max="2" width="29.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47" style="2" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="46.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="39.5703125" style="2" customWidth="1"/>
+    <col min="8" max="9" width="38.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="42" style="2" customWidth="1"/>
+    <col min="11" max="11" width="40.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="32.42578125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="33.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="34.28515625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="38.7109375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="32.5703125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="31.7109375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="32.7109375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="36.42578125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="33.28515625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="34" style="2" customWidth="1"/>
+    <col min="22" max="22" width="33.28515625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="38.7109375" style="2" customWidth="1"/>
+    <col min="24" max="24" width="34.42578125" style="2" customWidth="1"/>
+    <col min="25" max="25" width="33" style="2" customWidth="1"/>
+    <col min="26" max="26" width="33.85546875" style="2" customWidth="1"/>
+    <col min="27" max="27" width="32.85546875" style="2" customWidth="1"/>
+    <col min="28" max="28" width="36.42578125" style="2" customWidth="1"/>
+    <col min="29" max="29" width="32.7109375" style="2" customWidth="1"/>
+    <col min="30" max="30" width="32.5703125" style="2" customWidth="1"/>
+    <col min="31" max="31" width="37.28515625" style="2" customWidth="1"/>
+    <col min="32" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="2:48" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="2:48" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="AA2" s="2" t="s">
-        <v>422</v>
-      </c>
       <c r="AB2" s="2" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3" spans="2:48" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
@@ -2108,11 +2187,11 @@
         <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="H3" s="2" t="s">
         <v>15</v>
       </c>
@@ -2176,100 +2255,115 @@
       <c r="AB3" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="AC3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:48" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>56</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>50</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>144</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>221</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>50</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>200</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>242</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>200</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>250</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>144</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>266</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>275</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>285</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>221</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>305</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>329</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>200</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>350</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>358</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>367</v>
       </c>
-      <c r="AA4" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="AB4" t="s">
+        <v>423</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>329</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="2:48" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
@@ -2345,29 +2439,35 @@
       <c r="AB5" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="AC5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:48" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
         <v>70</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="H6" s="2" t="s">
         <v>19</v>
       </c>
@@ -2387,11 +2487,11 @@
         <v>19</v>
       </c>
       <c r="N6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="O6" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="P6" s="2" t="s">
         <v>19</v>
       </c>
@@ -2414,10 +2514,10 @@
         <v>19</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="Y6" s="2" t="s">
         <v>19</v>
@@ -2431,17 +2531,23 @@
       <c r="AB6" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:47" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="AC6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:48" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
@@ -2449,22 +2555,22 @@
         <v>13</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>413</v>
-      </c>
       <c r="K7" s="2" t="s">
-        <v>19</v>
+        <v>412</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>19</v>
@@ -2473,10 +2579,10 @@
         <v>19</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="P7" s="2" t="s">
         <v>19</v>
@@ -2494,7 +2600,7 @@
         <v>19</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="V7" s="2" t="s">
         <v>13</v>
@@ -2503,7 +2609,7 @@
         <v>13</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="Y7" s="2" t="s">
         <v>19</v>
@@ -2517,17 +2623,23 @@
       <c r="AB7" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:47" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="AC7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:48" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="D8" s="2" t="s">
         <v>19</v>
       </c>
@@ -2541,10 +2653,10 @@
         <v>19</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>19</v>
@@ -2603,108 +2715,120 @@
       <c r="AB8" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:47" ht="246" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="AC8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:48" ht="246" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="H9" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="I9" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="J9" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="K9" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="L9" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="M9" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="M9" s="7" t="s">
+      <c r="N9" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="N9" s="7" t="s">
+      <c r="O9" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="O9" s="7" t="s">
+      <c r="P9" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="P9" s="7" t="s">
+      <c r="Q9" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="Q9" s="7" t="s">
+      <c r="R9" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="R9" s="7" t="s">
+      <c r="S9" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="S9" s="7" t="s">
+      <c r="T9" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="T9" s="7" t="s">
+      <c r="U9" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="U9" s="7" t="s">
+      <c r="V9" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="V9" s="7" t="s">
+      <c r="W9" s="7" t="s">
         <v>334</v>
       </c>
-      <c r="W9" s="7" t="s">
+      <c r="X9" s="7" t="s">
         <v>344</v>
       </c>
-      <c r="X9" s="7" t="s">
+      <c r="Y9" s="7" t="s">
         <v>347</v>
       </c>
-      <c r="Y9" s="7" t="s">
+      <c r="Z9" s="7" t="s">
         <v>357</v>
       </c>
-      <c r="Z9" s="7" t="s">
+      <c r="AA9" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="AA9" s="7" t="s">
-        <v>428</v>
-      </c>
       <c r="AB9" s="7" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="10" spans="1:47" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="AC9" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="AD9" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="AE9" s="7" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="10" spans="2:48" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="D10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>19</v>
@@ -2716,22 +2840,22 @@
         <v>19</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="O10" s="2" t="s">
         <v>19</v>
@@ -2775,23 +2899,29 @@
       <c r="AB10" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:47" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="AC10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:48" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F11" s="2" t="s">
         <v>15</v>
       </c>
@@ -2802,23 +2932,23 @@
         <v>15</v>
       </c>
       <c r="I11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="L11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="M11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N11" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="N11" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="O11" s="2" t="s">
         <v>15</v>
       </c>
@@ -2861,23 +2991,29 @@
       <c r="AB11" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:47" ht="135" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="AC11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:48" ht="135" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F12" s="2" t="s">
         <v>15</v>
       </c>
@@ -2888,23 +3024,23 @@
         <v>15</v>
       </c>
       <c r="I12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="L12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="M12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N12" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="N12" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="O12" s="2" t="s">
         <v>15</v>
       </c>
@@ -2947,17 +3083,23 @@
       <c r="AB12" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:47" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="AC12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:48" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="D13" s="2" t="s">
         <v>13</v>
       </c>
@@ -2970,20 +3112,20 @@
       <c r="G13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="R13" s="2" t="s">
         <v>15</v>
@@ -2994,14 +3136,14 @@
       <c r="T13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="V13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="X13" s="2" t="s">
-        <v>19</v>
+      <c r="U13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="Y13" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="Z13" s="2" t="s">
         <v>13</v>
@@ -3012,22 +3154,28 @@
       <c r="AB13" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:47" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="AC13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE13" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:48" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="D14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>19</v>
@@ -3035,20 +3183,20 @@
       <c r="G14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" s="2" t="s">
-        <v>15</v>
+      <c r="M14" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="R14" s="2" t="s">
         <v>15</v>
@@ -3060,12 +3208,12 @@
         <v>15</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="V14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="X14" s="2" t="s">
+      <c r="W14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="Y14" s="2" t="s">
@@ -3080,19 +3228,25 @@
       <c r="AB14" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:47" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="AC14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE14" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="2:48" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>19</v>
@@ -3103,7 +3257,7 @@
       <c r="G15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J15" s="2" t="s">
@@ -3115,8 +3269,8 @@
       <c r="L15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="2" t="s">
-        <v>15</v>
+      <c r="M15" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="R15" s="2" t="s">
         <v>15</v>
@@ -3128,12 +3282,12 @@
         <v>15</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="V15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="X15" s="2" t="s">
+      <c r="W15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="Y15" s="2" t="s">
@@ -3148,43 +3302,49 @@
       <c r="AB15" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:47" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="AC15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE15" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="2:48" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="D16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q16" s="2" t="s">
-        <v>15</v>
+      <c r="M16" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="R16" s="2" t="s">
         <v>15</v>
@@ -3196,13 +3356,13 @@
         <v>15</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="X16" s="2" t="s">
-        <v>19</v>
+        <v>19</v>
+      </c>
+      <c r="W16" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="Y16" s="2" t="s">
         <v>19</v>
@@ -3214,105 +3374,114 @@
         <v>19</v>
       </c>
       <c r="AB16" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" ht="225" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE16" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:31" ht="225" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="J17" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="V17" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="W17" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="Y17" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="Z17" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="AB17" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="AE17" s="2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="18" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="S17" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="T17" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="U17" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="V17" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="X17" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="Y17" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="AA17" s="2" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="K18" s="2" t="s">
         <v>19</v>
       </c>
@@ -3323,26 +3492,26 @@
         <v>19</v>
       </c>
       <c r="N18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O18" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>255</v>
       </c>
       <c r="P18" s="2" t="s">
         <v>255</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>19</v>
+        <v>255</v>
       </c>
       <c r="R18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S18" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="S18" s="2" t="s">
+      <c r="T18" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="T18" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="U18" s="2" t="s">
         <v>19</v>
       </c>
@@ -3367,19 +3536,25 @@
       <c r="AB18" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:28" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="AC18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE18" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:31" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>19</v>
@@ -3390,11 +3565,11 @@
       <c r="G19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>411</v>
+      <c r="H19" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>19</v>
+        <v>410</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>19</v>
@@ -3406,26 +3581,26 @@
         <v>19</v>
       </c>
       <c r="N19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O19" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>255</v>
       </c>
       <c r="P19" s="2" t="s">
         <v>255</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>19</v>
+        <v>255</v>
       </c>
       <c r="R19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S19" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="S19" s="2" t="s">
+      <c r="T19" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="T19" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="U19" s="2" t="s">
         <v>19</v>
       </c>
@@ -3450,17 +3625,23 @@
       <c r="AB19" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="AC19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD19" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="AE19" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="D20" s="2" t="s">
         <v>19</v>
       </c>
@@ -3473,11 +3654,11 @@
       <c r="G20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>412</v>
+      <c r="H20" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>19</v>
+        <v>411</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>19</v>
@@ -3489,10 +3670,10 @@
         <v>19</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="P20" s="2" t="s">
         <v>19</v>
@@ -3533,52 +3714,58 @@
       <c r="AB20" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="AC20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE20" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="K21" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="L21" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="L21" s="2" t="s">
+      <c r="M21" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="N21" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="N21" s="2" t="s">
+      <c r="O21" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="P21" s="2" t="s">
         <v>236</v>
@@ -3596,60 +3783,66 @@
         <v>236</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>332</v>
+        <v>236</v>
       </c>
       <c r="V21" s="2" t="s">
         <v>332</v>
       </c>
       <c r="W21" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="X21" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="X21" s="2" t="s">
+      <c r="Y21" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="Y21" s="2" t="s">
+      <c r="Z21" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="Z21" s="2" t="s">
+      <c r="AA21" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="AA21" s="2" t="s">
-        <v>431</v>
-      </c>
       <c r="AB21" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="AC21" s="2" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="22" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="AD21" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="AE21" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>13</v>
@@ -3702,20 +3895,26 @@
       <c r="AB22" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="AC22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE22" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="E23" s="2" t="s">
         <v>19</v>
       </c>
@@ -3723,10 +3922,10 @@
         <v>19</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>19</v>
+        <v>19</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>19</v>
@@ -3741,11 +3940,11 @@
         <v>19</v>
       </c>
       <c r="N23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O23" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="O23" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="P23" s="2" t="s">
         <v>19</v>
       </c>
@@ -3762,10 +3961,10 @@
         <v>19</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="V23" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="W23" s="2" t="s">
         <v>19</v>
@@ -3785,17 +3984,23 @@
       <c r="AB23" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="AC23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE23" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="D24" s="2" t="s">
         <v>19</v>
       </c>
@@ -3808,7 +4013,7 @@
       <c r="G24" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J24" s="2" t="s">
@@ -3863,353 +4068,377 @@
         <v>19</v>
       </c>
       <c r="AA24" s="2" t="s">
-        <v>433</v>
+        <v>19</v>
       </c>
       <c r="AB24" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="AC24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE24" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="2:31" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="3"/>
+      <c r="G25" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G25" s="3"/>
-      <c r="I25" s="2" t="s">
+      <c r="H25" s="3"/>
+      <c r="J25" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="K25" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="M25" s="2" t="s">
+      <c r="N25" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>260</v>
       </c>
       <c r="Q25" s="2" t="s">
         <v>260</v>
       </c>
       <c r="R25" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="S25" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="S25" s="3" t="s">
+      <c r="T25" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="T25" s="3" t="s">
+      <c r="U25" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="V25" s="2" t="s">
+      <c r="W25" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="W25" s="2" t="s">
+      <c r="X25" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="Y25" s="3" t="s">
+      <c r="Z25" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="Z25" s="3" t="s">
+      <c r="AA25" s="3" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="26" spans="1:28" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="AD25" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="AE25" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="26" spans="2:31" ht="45" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="H26" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="I26" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="J26" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="J26" s="12" t="s">
+      <c r="K26" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="K26" s="3" t="s">
+      <c r="L26" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="L26" s="3" t="s">
+      <c r="M26" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="M26" s="3" t="s">
+      <c r="N26" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="N26" s="3" t="s">
+      <c r="O26" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="O26" s="2" t="s">
+      <c r="P26" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="P26" s="3" t="s">
+      <c r="Q26" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="Q26" s="3" t="s">
+      <c r="R26" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="R26" s="3" t="s">
+      <c r="S26" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="S26" s="3" t="s">
+      <c r="T26" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="T26" s="2" t="s">
+      <c r="U26" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="U26" s="3" t="s">
+      <c r="V26" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="V26" s="3" t="s">
+      <c r="W26" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="X26" s="3" t="s">
+      <c r="Y26" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="Z26" s="3" t="s">
+      <c r="AA26" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="AA26" s="3" t="s">
+      <c r="AB26" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="AC26" s="3" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="27" spans="2:31" ht="60" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="R27" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="U27" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="V27" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="W27" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="X27" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="Y27" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="Z27" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="AB27" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="AD27" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="AE27" s="2" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="28" spans="2:31" ht="45" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="K28" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="O28" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="P28" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q28" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="R28" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="S28" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="T28" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="U28" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="V28" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="W28" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="X28" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="Z28" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="AA28" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="AB28" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="AB26" s="3" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="I27" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q27" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="T27" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="U27" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="V27" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="W27" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="X27" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="Y27" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="AA27" s="3" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="J28" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="N28" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="O28" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="P28" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="Q28" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="R28" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="S28" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="T28" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="U28" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="V28" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="W28" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="Y28" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="Z28" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="AA28" s="3" t="s">
-        <v>426</v>
-      </c>
-      <c r="AB28" s="3" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" ht="45" x14ac:dyDescent="0.25">
-      <c r="C29" s="3" t="s">
+      <c r="AC28" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="AD28" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="AE28" s="2" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="29" spans="2:31" ht="45" x14ac:dyDescent="0.25">
+      <c r="D29" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="3"/>
+      <c r="F29" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F29" s="3"/>
-      <c r="I29" s="3" t="s">
+      <c r="G29" s="3"/>
+      <c r="J29" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="W29" s="3" t="s">
+      <c r="X29" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="Z29" s="3" t="s">
+      <c r="AA29" s="3" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="30" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="2:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G31" t="s">
         <v>142</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>74</v>
       </c>
-      <c r="H31" s="13" t="s">
+      <c r="I31" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="J31" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="K31" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="L31" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="L31" s="2" t="s">
+      <c r="M31" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="M31" s="2" t="s">
+      <c r="N31" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>231</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="P31" s="2" t="s">
         <v>151</v>
@@ -4223,8 +4452,8 @@
       <c r="S31" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="T31" s="5" t="s">
-        <v>231</v>
+      <c r="T31" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="U31" s="5" t="s">
         <v>231</v>
@@ -4233,566 +4462,641 @@
         <v>231</v>
       </c>
       <c r="W31" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="X31" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="X31" s="2" t="s">
+      <c r="Y31" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="Y31" t="s">
+      <c r="Z31" t="s">
         <v>142</v>
       </c>
-      <c r="Z31" s="2" t="s">
+      <c r="AA31" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="AA31" s="2" t="s">
+      <c r="AB31" s="2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+      <c r="AD31" t="s">
+        <v>231</v>
+      </c>
+      <c r="AE31" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B32" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="14">
+      <c r="D32" s="14">
         <v>44222</v>
       </c>
-      <c r="D32" s="14">
+      <c r="E32" s="14">
         <v>42737</v>
       </c>
-      <c r="E32" s="15">
+      <c r="F32" s="15">
         <v>41862</v>
       </c>
-      <c r="F32" s="15">
+      <c r="G32" s="15">
         <v>41193</v>
       </c>
-      <c r="G32" s="15">
+      <c r="H32" s="15">
         <v>43217</v>
       </c>
-      <c r="H32" s="15">
+      <c r="I32" s="15">
         <v>42836</v>
       </c>
-      <c r="I32" s="15">
+      <c r="J32" s="15">
         <v>42248</v>
       </c>
-      <c r="J32" s="15">
+      <c r="K32" s="15">
         <v>42908</v>
       </c>
-      <c r="K32" s="15">
+      <c r="L32" s="15">
         <v>42454</v>
       </c>
-      <c r="L32" s="15">
+      <c r="M32" s="15">
         <v>41538</v>
       </c>
-      <c r="M32" s="15">
+      <c r="N32" s="15">
         <v>41518</v>
       </c>
-      <c r="N32" s="15">
+      <c r="O32" s="15">
         <v>41380</v>
       </c>
-      <c r="O32" s="15">
+      <c r="P32" s="15">
         <v>40604</v>
       </c>
-      <c r="P32" s="15">
+      <c r="Q32" s="15">
         <v>42441</v>
       </c>
-      <c r="Q32" s="15">
+      <c r="R32" s="15">
         <v>43014</v>
       </c>
-      <c r="R32" s="15">
+      <c r="S32" s="15">
         <v>40574</v>
       </c>
-      <c r="S32" s="15">
+      <c r="T32" s="15">
         <v>42734</v>
       </c>
-      <c r="T32" s="14">
+      <c r="U32" s="14">
         <v>42646</v>
       </c>
-      <c r="U32" s="14">
+      <c r="V32" s="14">
         <v>42430</v>
       </c>
-      <c r="V32" s="14">
+      <c r="W32" s="14">
         <v>43196</v>
       </c>
-      <c r="W32" s="14">
+      <c r="X32" s="14">
         <v>42441</v>
       </c>
-      <c r="X32" s="14">
+      <c r="Y32" s="14">
         <v>42410</v>
       </c>
-      <c r="Y32" s="14">
+      <c r="Z32" s="14">
         <v>37819</v>
       </c>
-      <c r="Z32" s="14">
+      <c r="AA32" s="14">
         <v>41058</v>
       </c>
-      <c r="AA32" s="14">
+      <c r="AB32" s="14">
         <v>42734</v>
       </c>
-    </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="AC32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD32" s="14">
+        <v>43231</v>
+      </c>
+      <c r="AE32" s="14">
+        <v>43601</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B33" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="14">
+      <c r="D33" s="14">
         <v>44442</v>
       </c>
-      <c r="D33" s="15">
+      <c r="E33" s="15">
         <v>44179</v>
       </c>
-      <c r="E33" s="15">
+      <c r="F33" s="15">
         <v>44405</v>
       </c>
-      <c r="F33" s="15">
+      <c r="G33" s="15">
         <v>44399</v>
       </c>
-      <c r="G33" s="15">
+      <c r="H33" s="15">
         <v>44441</v>
       </c>
-      <c r="H33" s="15">
+      <c r="I33" s="15">
         <v>43468</v>
       </c>
-      <c r="I33" s="15">
+      <c r="J33" s="15">
         <v>44476</v>
       </c>
-      <c r="J33" s="15">
+      <c r="K33" s="15">
         <v>42908</v>
       </c>
-      <c r="K33" s="15">
+      <c r="L33" s="15">
         <v>42454</v>
       </c>
-      <c r="L33" s="15">
+      <c r="M33" s="15">
         <v>41538</v>
       </c>
-      <c r="M33" s="15">
+      <c r="N33" s="15">
         <v>42606</v>
       </c>
-      <c r="N33" s="15">
+      <c r="O33" s="15">
         <v>42112</v>
       </c>
-      <c r="O33" s="15">
+      <c r="P33" s="15">
         <v>42200</v>
       </c>
-      <c r="P33" s="15">
+      <c r="Q33" s="15">
         <v>44284</v>
       </c>
-      <c r="Q33" s="15">
+      <c r="R33" s="15">
         <v>44463</v>
       </c>
-      <c r="R33" s="15">
+      <c r="S33" s="15">
         <v>43282</v>
       </c>
-      <c r="S33" s="15">
+      <c r="T33" s="15">
         <v>44319</v>
       </c>
-      <c r="T33" s="14">
+      <c r="U33" s="14">
         <v>44201</v>
       </c>
-      <c r="U33" s="14">
+      <c r="V33" s="14">
         <v>44180</v>
       </c>
-      <c r="V33" s="14">
+      <c r="W33" s="14">
         <v>44352</v>
       </c>
-      <c r="W33" s="14">
+      <c r="X33" s="14">
         <v>43357</v>
       </c>
-      <c r="X33" s="14">
+      <c r="Y33" s="14">
         <v>42410</v>
       </c>
-      <c r="Y33" s="14">
+      <c r="Z33" s="14">
         <v>44476</v>
       </c>
-      <c r="Z33" s="14">
+      <c r="AA33" s="14">
         <v>44044</v>
       </c>
-      <c r="AA33" s="14">
+      <c r="AB33" s="14">
         <v>44351</v>
       </c>
-    </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="AC33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD33" s="14">
+        <v>44171</v>
+      </c>
+      <c r="AE33" s="14">
+        <v>44351</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="D34" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="E34" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="G34" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="H34" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="I34" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="J34" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="K34" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>119</v>
       </c>
       <c r="M34" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="N34" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="N34" s="2" t="s">
+      <c r="O34" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="O34" s="2" t="s">
+      <c r="P34" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="P34" s="2" t="s">
+      <c r="Q34" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="Q34" s="2" t="s">
+      <c r="R34" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="R34" s="2" t="s">
+      <c r="S34" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="S34" s="2" t="s">
+      <c r="T34" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="T34" s="2" t="s">
+      <c r="U34" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="U34" s="5" t="s">
+      <c r="V34" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="V34" t="s">
+      <c r="W34" t="s">
         <v>326</v>
       </c>
-      <c r="W34" s="2">
+      <c r="X34" s="2">
         <v>1.2</v>
       </c>
-      <c r="X34" s="2">
+      <c r="Y34" s="2">
         <v>0.1</v>
       </c>
-      <c r="Y34" t="s">
+      <c r="Z34" t="s">
         <v>359</v>
       </c>
-      <c r="Z34" t="s">
+      <c r="AA34" t="s">
         <v>370</v>
       </c>
-      <c r="AA34" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="36" spans="1:28" ht="126" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="AB34" t="s">
+        <v>422</v>
+      </c>
+      <c r="AC34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD34" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="E36" s="5" t="s">
         <v>402</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="F36" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="G36" s="6" t="s">
+      <c r="H36" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="V36" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="W36" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="Z36" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="AC36" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="AD36" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="AE36" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" ht="75" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="F37" s="6"/>
+      <c r="I37" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="O37" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="R37" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="S37" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="T37" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="U37" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="W37" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="X37" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="Y37" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="Z37" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="AC37" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D39" s="9"/>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B41" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>1</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="AB42" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>2</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="AA43" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="AB43" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="AC43" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="AD43" s="2" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>3</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="U44" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="AA44" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>4</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="W45" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="AA45" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>5</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="W46" s="2" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>6</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="H47" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="J36" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="U36" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="V36" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="Y36" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="AB36" s="2" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="37" spans="1:28" ht="75" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>400</v>
-      </c>
-      <c r="E37" s="6"/>
-      <c r="H37" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="L37" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="M37" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="N37" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="O37" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="P37" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="Q37" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="R37" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="S37" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="T37" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="V37" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="W37" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="X37" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="Y37" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="AB37" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C39" s="9"/>
-    </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="AA42" s="2" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="Z43" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="AA43" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="AB43" s="2" t="s">
+      <c r="J47" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="W47" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="Z47" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="AA47" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="AC47" s="2" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="T44" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="Z44" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="V45" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="Z45" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="V46" s="2" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="V47" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="Y47" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="Z47" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="AB47" s="2" t="s">
+      <c r="AE47" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>7</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>8</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="E50" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="W50" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="Z50" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="AC50" s="2" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="48" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="D50" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="L50" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="V50" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="Y50" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="AB50" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="51" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="D51" s="2" t="s">
+      <c r="AE50" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="51" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="E51" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="I51" s="2" t="s">
+      <c r="J51" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="52" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="D52" s="2" t="s">
+    <row r="52" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="E52" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="I52" s="2" t="s">
+      <c r="J52" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="I53" s="2" t="s">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="J53" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B54" s="11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+    <row r="55" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>9</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>125</v>
@@ -4801,387 +5105,512 @@
         <v>125</v>
       </c>
       <c r="G55" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H55" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="I55" s="2" t="s">
+      <c r="J55" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="J55" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="L55" s="2" t="s">
+      <c r="K55" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="M55" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="U55" s="2" t="s">
+      <c r="V55" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="V55" s="2" t="s">
+      <c r="W55" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="Y55" s="2" t="s">
+      <c r="Z55" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="Z55" s="2" t="s">
+      <c r="AA55" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="AA55" s="2" t="s">
-        <v>430</v>
-      </c>
       <c r="AB55" s="2" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="AC55" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="AE55" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>10</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>11</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>12</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="59" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+    <row r="59" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>13</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="J59" s="2" t="s">
+      <c r="K59" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B61" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="62" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+    <row r="62" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>14</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="I62" s="2" t="s">
+      <c r="J62" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>15</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="I63" s="2" t="s">
+      <c r="J63" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="64" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+    <row r="64" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>16</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I64" s="2" t="s">
+      <c r="J64" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="65" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+    <row r="65" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>17</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>18</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="67" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+    <row r="67" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>19</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="I67" s="2" t="s">
+      <c r="J67" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>20</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="I68" s="2" t="s">
+      <c r="J68" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="69" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+    <row r="69" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>21</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="D69" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="I69" s="2" t="s">
+      <c r="J69" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>22</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="D70" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="I71" s="2" t="s">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="J71" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A73" s="11" t="s">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B73" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+    <row r="74" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>23</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="D74" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="E74" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="H74" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="J74" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="V74" s="2" t="s">
+      <c r="K74" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="W74" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="AB74" s="2" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+      <c r="AC74" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="AD74" t="s">
+        <v>449</v>
+      </c>
+      <c r="AE74" s="2" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="75" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>24</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="D75" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>25</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="D76" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>26</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="D77" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>405</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="J77" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="U77" s="2" t="s">
-        <v>415</v>
+      <c r="F77" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="K77" s="2" t="s">
+        <v>414</v>
       </c>
       <c r="V77" s="2" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="W77" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="AD77" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="AE77" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="78" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>27</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>28</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
+    <row r="80" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>29</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="D80" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="U80" s="2" t="s">
+      <c r="H80" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="V80" s="2" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="81" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
+      <c r="AD80" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="AE80" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="81" spans="1:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>30</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="D81" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="U81" s="2" t="s">
+      <c r="H81" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="V81" s="2" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
+      <c r="AD81" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="AE81" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="82" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>31</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="D82" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
+      <c r="H82" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="AD82" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="AE82" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="83" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>32</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>33</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="D84" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="85" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+    <row r="85" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>34</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="D85" s="2" t="s">
         <v>116</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C28" r:id="rId1"/>
-    <hyperlink ref="C27" r:id="rId2"/>
-    <hyperlink ref="C26" r:id="rId3"/>
-    <hyperlink ref="C29" r:id="rId4"/>
-    <hyperlink ref="D27" r:id="rId5"/>
-    <hyperlink ref="D28" r:id="rId6"/>
-    <hyperlink ref="E28" r:id="rId7"/>
-    <hyperlink ref="E29" r:id="rId8"/>
-    <hyperlink ref="E27" r:id="rId9"/>
-    <hyperlink ref="F27" r:id="rId10"/>
-    <hyperlink ref="F28" r:id="rId11"/>
-    <hyperlink ref="F26" r:id="rId12"/>
-    <hyperlink ref="D26" r:id="rId13"/>
-    <hyperlink ref="E26" r:id="rId14"/>
-    <hyperlink ref="G26" r:id="rId15"/>
-    <hyperlink ref="I26" r:id="rId16"/>
-    <hyperlink ref="I27" r:id="rId17"/>
-    <hyperlink ref="I28" r:id="rId18"/>
-    <hyperlink ref="I29" r:id="rId19"/>
-    <hyperlink ref="J26" r:id="rId20"/>
-    <hyperlink ref="J27" r:id="rId21"/>
-    <hyperlink ref="J28" r:id="rId22"/>
-    <hyperlink ref="K26" r:id="rId23"/>
-    <hyperlink ref="K27" r:id="rId24"/>
-    <hyperlink ref="K28" r:id="rId25"/>
-    <hyperlink ref="L26" r:id="rId26"/>
-    <hyperlink ref="L28" r:id="rId27"/>
-    <hyperlink ref="M26" r:id="rId28"/>
-    <hyperlink ref="H26" r:id="rId29"/>
-    <hyperlink ref="H27" r:id="rId30"/>
-    <hyperlink ref="H28" r:id="rId31"/>
-    <hyperlink ref="N28" r:id="rId32"/>
-    <hyperlink ref="N26" r:id="rId33"/>
-    <hyperlink ref="O28" r:id="rId34"/>
-    <hyperlink ref="P26" r:id="rId35"/>
-    <hyperlink ref="P28" r:id="rId36"/>
-    <hyperlink ref="Q28" r:id="rId37"/>
-    <hyperlink ref="Q26" r:id="rId38"/>
-    <hyperlink ref="Q27" r:id="rId39"/>
-    <hyperlink ref="R26" r:id="rId40"/>
-    <hyperlink ref="R28" r:id="rId41"/>
-    <hyperlink ref="S26" r:id="rId42"/>
-    <hyperlink ref="S28" r:id="rId43"/>
-    <hyperlink ref="S25" r:id="rId44"/>
-    <hyperlink ref="T28" r:id="rId45"/>
-    <hyperlink ref="T27" r:id="rId46"/>
-    <hyperlink ref="T25" r:id="rId47"/>
-    <hyperlink ref="U26" r:id="rId48"/>
-    <hyperlink ref="U28" r:id="rId49"/>
-    <hyperlink ref="U27" r:id="rId50"/>
-    <hyperlink ref="V26" r:id="rId51"/>
-    <hyperlink ref="V28" r:id="rId52"/>
-    <hyperlink ref="V27" r:id="rId53"/>
-    <hyperlink ref="W28" r:id="rId54"/>
-    <hyperlink ref="W29" r:id="rId55"/>
-    <hyperlink ref="W27" r:id="rId56"/>
-    <hyperlink ref="X27" r:id="rId57"/>
-    <hyperlink ref="X26" r:id="rId58"/>
-    <hyperlink ref="Y28" r:id="rId59"/>
-    <hyperlink ref="Y27" r:id="rId60"/>
-    <hyperlink ref="Y25" r:id="rId61"/>
-    <hyperlink ref="Z25" r:id="rId62"/>
-    <hyperlink ref="Z28" r:id="rId63"/>
-    <hyperlink ref="Z26" r:id="rId64"/>
-    <hyperlink ref="Z29" r:id="rId65"/>
-    <hyperlink ref="AA26" r:id="rId66"/>
-    <hyperlink ref="AA28" r:id="rId67"/>
-    <hyperlink ref="AA27" r:id="rId68"/>
-    <hyperlink ref="AA42" r:id="rId69" display="https://mayoverse.github.io/arsenal/reference/comparedf.html"/>
-    <hyperlink ref="AA43" r:id="rId70" display="https://mayoverse.github.io/arsenal/reference/comparedf.html"/>
-    <hyperlink ref="AB28" r:id="rId71"/>
-    <hyperlink ref="AB26" r:id="rId72"/>
+    <hyperlink ref="D28" r:id="rId1"/>
+    <hyperlink ref="D27" r:id="rId2"/>
+    <hyperlink ref="D26" r:id="rId3"/>
+    <hyperlink ref="D29" r:id="rId4"/>
+    <hyperlink ref="E27" r:id="rId5"/>
+    <hyperlink ref="E28" r:id="rId6"/>
+    <hyperlink ref="F28" r:id="rId7"/>
+    <hyperlink ref="F29" r:id="rId8"/>
+    <hyperlink ref="F27" r:id="rId9"/>
+    <hyperlink ref="G27" r:id="rId10"/>
+    <hyperlink ref="G28" r:id="rId11"/>
+    <hyperlink ref="G26" r:id="rId12"/>
+    <hyperlink ref="E26" r:id="rId13"/>
+    <hyperlink ref="F26" r:id="rId14"/>
+    <hyperlink ref="H26" r:id="rId15"/>
+    <hyperlink ref="J26" r:id="rId16"/>
+    <hyperlink ref="J27" r:id="rId17"/>
+    <hyperlink ref="J28" r:id="rId18"/>
+    <hyperlink ref="J29" r:id="rId19"/>
+    <hyperlink ref="K26" r:id="rId20"/>
+    <hyperlink ref="K27" r:id="rId21"/>
+    <hyperlink ref="K28" r:id="rId22"/>
+    <hyperlink ref="L26" r:id="rId23"/>
+    <hyperlink ref="L27" r:id="rId24"/>
+    <hyperlink ref="L28" r:id="rId25"/>
+    <hyperlink ref="M26" r:id="rId26"/>
+    <hyperlink ref="M28" r:id="rId27"/>
+    <hyperlink ref="N26" r:id="rId28"/>
+    <hyperlink ref="I26" r:id="rId29"/>
+    <hyperlink ref="I27" r:id="rId30"/>
+    <hyperlink ref="I28" r:id="rId31"/>
+    <hyperlink ref="O28" r:id="rId32"/>
+    <hyperlink ref="O26" r:id="rId33"/>
+    <hyperlink ref="P28" r:id="rId34"/>
+    <hyperlink ref="Q26" r:id="rId35"/>
+    <hyperlink ref="Q28" r:id="rId36"/>
+    <hyperlink ref="R28" r:id="rId37"/>
+    <hyperlink ref="R26" r:id="rId38"/>
+    <hyperlink ref="R27" r:id="rId39"/>
+    <hyperlink ref="S26" r:id="rId40"/>
+    <hyperlink ref="S28" r:id="rId41"/>
+    <hyperlink ref="T26" r:id="rId42"/>
+    <hyperlink ref="T28" r:id="rId43"/>
+    <hyperlink ref="T25" r:id="rId44"/>
+    <hyperlink ref="U28" r:id="rId45"/>
+    <hyperlink ref="U27" r:id="rId46"/>
+    <hyperlink ref="U25" r:id="rId47"/>
+    <hyperlink ref="V26" r:id="rId48"/>
+    <hyperlink ref="V28" r:id="rId49"/>
+    <hyperlink ref="V27" r:id="rId50"/>
+    <hyperlink ref="W26" r:id="rId51"/>
+    <hyperlink ref="W28" r:id="rId52"/>
+    <hyperlink ref="W27" r:id="rId53"/>
+    <hyperlink ref="X28" r:id="rId54"/>
+    <hyperlink ref="X29" r:id="rId55"/>
+    <hyperlink ref="X27" r:id="rId56"/>
+    <hyperlink ref="Y27" r:id="rId57"/>
+    <hyperlink ref="Y26" r:id="rId58"/>
+    <hyperlink ref="Z28" r:id="rId59"/>
+    <hyperlink ref="Z27" r:id="rId60"/>
+    <hyperlink ref="Z25" r:id="rId61"/>
+    <hyperlink ref="AA25" r:id="rId62"/>
+    <hyperlink ref="AA28" r:id="rId63"/>
+    <hyperlink ref="AA26" r:id="rId64"/>
+    <hyperlink ref="AA29" r:id="rId65"/>
+    <hyperlink ref="AB26" r:id="rId66"/>
+    <hyperlink ref="AB28" r:id="rId67"/>
+    <hyperlink ref="AB27" r:id="rId68"/>
+    <hyperlink ref="AB42" r:id="rId69" display="https://mayoverse.github.io/arsenal/reference/comparedf.html"/>
+    <hyperlink ref="AB43" r:id="rId70" display="https://mayoverse.github.io/arsenal/reference/comparedf.html"/>
+    <hyperlink ref="AC28" r:id="rId71"/>
+    <hyperlink ref="AC26" r:id="rId72"/>
+    <hyperlink ref="AD27" r:id="rId73"/>
+    <hyperlink ref="AD28" r:id="rId74"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId73"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add inspectdf + visdat
</commit_message>
<xml_diff>
--- a/Data quality revision R overview v01.xlsx
+++ b/Data quality revision R overview v01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="2670" tabRatio="169"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="2676" tabRatio="169"/>
   </bookViews>
   <sheets>
     <sheet name="Tools" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="507">
   <si>
     <t>Acronym (falls vorhanden)</t>
   </si>
@@ -1538,6 +1538,73 @@
   </si>
   <si>
     <t>R objects, jpg</t>
+  </si>
+  <si>
+    <t>inspectdf</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=inspectdf</t>
+  </si>
+  <si>
+    <t>0.0.11</t>
+  </si>
+  <si>
+    <t>https://alastairrushworth.github.io/inspectdf/</t>
+  </si>
+  <si>
+    <t>https://github.com/alastairrushworth/inspectdf/</t>
+  </si>
+  <si>
+    <t>inspect_types</t>
+  </si>
+  <si>
+    <t>Number of columns</t>
+  </si>
+  <si>
+    <t>Memory usage per column. Comparison across dataframes for all features.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min, q1, mean, median,q3, max, sd, histogram </t>
+  </si>
+  <si>
+    <t>inspect_cor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A collection of utilities for columnwise summary, comparison and visualisation of data frames. Functions report missingness, categorical levels, numeric distribution, correlation, column types and memory usage. The package has three aims:
+    to speed up repetitive checking and exploratory tasks for data frames
+    to make it easier to compare data frames for differences and inconsistencies
+    to support quick visualisation of data frames
+</t>
+  </si>
+  <si>
+    <t>visdat</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=visdat</t>
+  </si>
+  <si>
+    <t>≥ 3.2.2</t>
+  </si>
+  <si>
+    <t>https://github.com/ropensci/visdat</t>
+  </si>
+  <si>
+    <t>https://docs.ropensci.org/visdat/</t>
+  </si>
+  <si>
+    <t>Create preliminary exploratory data visualisations of an entire dataset to identify problems or unexpected features using 'ggplot2'.</t>
+  </si>
+  <si>
+    <t>No of variables</t>
+  </si>
+  <si>
+    <t>No of observations</t>
+  </si>
+  <si>
+    <t>vis_cor</t>
+  </si>
+  <si>
+    <t>Compare datasets of the same size. Visualise the values of the data on a 0 to 1 scale, or binary values</t>
   </si>
 </sst>
 </file>
@@ -1956,46 +2023,48 @@
   <dimension ref="A1:AV86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="AE27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="AG3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AF29" sqref="AF29"/>
+      <selection pane="bottomRight" activeCell="AH9" sqref="AH9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11" style="2"/>
-    <col min="2" max="2" width="29.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="47" style="2" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="46.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="39.5703125" style="2" customWidth="1"/>
-    <col min="8" max="9" width="38.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="43.88671875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="46.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="39.5546875" style="2" customWidth="1"/>
+    <col min="8" max="9" width="38.6640625" style="2" customWidth="1"/>
     <col min="10" max="10" width="42" style="2" customWidth="1"/>
-    <col min="11" max="11" width="40.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="32.42578125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="33.7109375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="34.28515625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="38.7109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="32.5703125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="31.7109375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="32.7109375" style="2" customWidth="1"/>
-    <col min="19" max="19" width="36.42578125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="33.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="40.44140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="32.44140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="33.6640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="34.33203125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="38.6640625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="32.5546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="31.6640625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="32.6640625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="36.44140625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="33.33203125" style="2" customWidth="1"/>
     <col min="21" max="21" width="34" style="2" customWidth="1"/>
-    <col min="22" max="22" width="33.28515625" style="2" customWidth="1"/>
-    <col min="23" max="23" width="38.7109375" style="2" customWidth="1"/>
-    <col min="24" max="24" width="34.42578125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="33.33203125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="38.6640625" style="2" customWidth="1"/>
+    <col min="24" max="24" width="34.44140625" style="2" customWidth="1"/>
     <col min="25" max="25" width="33" style="2" customWidth="1"/>
-    <col min="26" max="26" width="33.85546875" style="2" customWidth="1"/>
-    <col min="27" max="27" width="32.85546875" style="2" customWidth="1"/>
-    <col min="28" max="28" width="36.42578125" style="2" customWidth="1"/>
-    <col min="29" max="29" width="32.7109375" style="2" customWidth="1"/>
-    <col min="30" max="30" width="32.5703125" style="2" customWidth="1"/>
-    <col min="31" max="31" width="37.28515625" style="2" customWidth="1"/>
-    <col min="32" max="32" width="38.42578125" style="2" customWidth="1"/>
-    <col min="33" max="16384" width="11" style="2"/>
+    <col min="26" max="26" width="33.88671875" style="2" customWidth="1"/>
+    <col min="27" max="27" width="32.88671875" style="2" customWidth="1"/>
+    <col min="28" max="28" width="36.44140625" style="2" customWidth="1"/>
+    <col min="29" max="29" width="32.6640625" style="2" customWidth="1"/>
+    <col min="30" max="30" width="32.5546875" style="2" customWidth="1"/>
+    <col min="31" max="31" width="37.33203125" style="2" customWidth="1"/>
+    <col min="32" max="32" width="38.44140625" style="2" customWidth="1"/>
+    <col min="33" max="33" width="33.109375" style="2" customWidth="1"/>
+    <col min="34" max="34" width="32.88671875" style="2" customWidth="1"/>
+    <col min="35" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:48" s="4" customFormat="1">
@@ -2235,6 +2304,12 @@
       <c r="AF2" s="2" t="s">
         <v>469</v>
       </c>
+      <c r="AG2" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>497</v>
+      </c>
     </row>
     <row r="3" spans="2:48">
       <c r="B3" s="2" t="s">
@@ -2330,6 +2405,12 @@
       <c r="AF3" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="AG3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="2:48">
       <c r="B4" s="2" t="s">
@@ -2425,6 +2506,12 @@
       <c r="AF4" s="2" t="s">
         <v>471</v>
       </c>
+      <c r="AG4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="5" spans="2:48">
       <c r="B5" s="8" t="s">
@@ -2520,6 +2607,12 @@
       <c r="AF5" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="AG5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH5" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="2:48">
       <c r="B6" s="2" t="s">
@@ -2615,8 +2708,14 @@
       <c r="AF6" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="2:48" ht="45">
+      <c r="AG6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:48" ht="28.8">
       <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
@@ -2710,8 +2809,14 @@
       <c r="AF7" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="2:48" ht="30">
+      <c r="AG7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:48" ht="28.8">
       <c r="B8" s="2" t="s">
         <v>40</v>
       </c>
@@ -2803,6 +2908,12 @@
         <v>19</v>
       </c>
       <c r="AF8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH8" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2897,11 +3008,17 @@
       <c r="AE9" s="7" t="s">
         <v>457</v>
       </c>
-      <c r="AF9" s="2" t="s">
+      <c r="AF9" s="7" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="10" spans="2:48" ht="30">
+      <c r="AG9" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="AH9" s="7" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="10" spans="2:48">
       <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
@@ -2995,8 +3112,14 @@
       <c r="AF10" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="2:48" ht="30">
+      <c r="AG10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:48" ht="28.8">
       <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
@@ -3090,8 +3213,14 @@
       <c r="AF11" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="2:48" ht="135">
+      <c r="AG11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:48" ht="115.2">
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
@@ -3183,6 +3312,12 @@
         <v>15</v>
       </c>
       <c r="AF12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH12" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3259,8 +3394,14 @@
       <c r="AF13" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="2:48" ht="30">
+      <c r="AG13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH13" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:48" ht="28.8">
       <c r="B14" s="2" t="s">
         <v>45</v>
       </c>
@@ -3336,8 +3477,14 @@
       <c r="AF14" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="2:48" ht="30">
+      <c r="AG14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:48" ht="28.8">
       <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
@@ -3411,6 +3558,12 @@
         <v>19</v>
       </c>
       <c r="AF15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH15" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3490,8 +3643,14 @@
       <c r="AF16" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="2:32" ht="225">
+      <c r="AG16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH16" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:37" ht="201.6">
       <c r="B17" s="2" t="s">
         <v>44</v>
       </c>
@@ -3564,8 +3723,14 @@
       <c r="AF17" s="2" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="18" spans="2:32" ht="30">
+      <c r="AG17" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="AH17" s="2" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="18" spans="2:37" ht="28.8">
       <c r="B18" s="2" t="s">
         <v>27</v>
       </c>
@@ -3656,8 +3821,14 @@
       <c r="AF18" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="2:32" ht="45">
+      <c r="AG18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH18" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:37" ht="28.8">
       <c r="B19" s="2" t="s">
         <v>28</v>
       </c>
@@ -3748,8 +3919,14 @@
       <c r="AF19" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="2:32" ht="30">
+      <c r="AG19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH19" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:37" ht="28.8">
       <c r="B20" s="2" t="s">
         <v>29</v>
       </c>
@@ -3840,8 +4017,14 @@
       <c r="AF20" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="2:32">
+      <c r="AG20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH20" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:37">
       <c r="B21" s="2" t="s">
         <v>30</v>
       </c>
@@ -3935,8 +4118,14 @@
       <c r="AF21" s="2" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="22" spans="2:32" ht="30">
+      <c r="AG21" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="AH21" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="22" spans="2:37" ht="28.8">
       <c r="B22" s="2" t="s">
         <v>35</v>
       </c>
@@ -4027,8 +4216,14 @@
       <c r="AF22" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="2:32">
+      <c r="AG22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH22" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="2:37">
       <c r="B23" s="2" t="s">
         <v>37</v>
       </c>
@@ -4119,8 +4314,14 @@
       <c r="AF23" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="2:32" ht="30">
+      <c r="AG23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH23" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="2:37" ht="28.8">
       <c r="B24" s="2" t="s">
         <v>39</v>
       </c>
@@ -4211,8 +4412,14 @@
       <c r="AF24" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="2:32" ht="90" customHeight="1">
+      <c r="AG24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH24" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="2:37" ht="90" customHeight="1">
       <c r="B25" s="2" t="s">
         <v>31</v>
       </c>
@@ -4275,8 +4482,14 @@
       <c r="AF25" s="2" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="26" spans="2:32" ht="45">
+      <c r="AG25" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="AH25" s="3" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="26" spans="2:37" ht="43.2">
       <c r="B26" s="2" t="s">
         <v>137</v>
       </c>
@@ -4356,7 +4569,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="27" spans="2:32" ht="60">
+    <row r="27" spans="2:37" ht="43.2">
       <c r="B27" s="2" t="s">
         <v>3</v>
       </c>
@@ -4423,8 +4636,14 @@
       <c r="AF27" s="2" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="28" spans="2:32" ht="45">
+      <c r="AG27" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="AH27" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="28" spans="2:37" ht="28.8">
       <c r="B28" s="2" t="s">
         <v>32</v>
       </c>
@@ -4512,8 +4731,14 @@
       <c r="AF28" s="2" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="29" spans="2:32" ht="45">
+      <c r="AG28" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="AH28" s="3" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="29" spans="2:37" ht="43.2">
       <c r="D29" s="3" t="s">
         <v>140</v>
       </c>
@@ -4532,10 +4757,10 @@
         <v>375</v>
       </c>
     </row>
-    <row r="30" spans="2:32">
+    <row r="30" spans="2:37">
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="2:32" ht="30">
+    <row r="31" spans="2:37">
       <c r="B31" s="2" t="s">
         <v>33</v>
       </c>
@@ -4626,8 +4851,14 @@
       <c r="AF31" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="32" spans="2:32">
+      <c r="AG31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH31" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="32" spans="2:37">
       <c r="B32" s="8" t="s">
         <v>78</v>
       </c>
@@ -4718,8 +4949,18 @@
       <c r="AE32" s="14">
         <v>43601</v>
       </c>
-    </row>
-    <row r="33" spans="1:32">
+      <c r="AF32" s="14"/>
+      <c r="AG32" s="14">
+        <v>43579</v>
+      </c>
+      <c r="AH32" s="14">
+        <v>42927</v>
+      </c>
+      <c r="AI32" s="14"/>
+      <c r="AJ32" s="14"/>
+      <c r="AK32" s="14"/>
+    </row>
+    <row r="33" spans="1:37">
       <c r="B33" s="8" t="s">
         <v>118</v>
       </c>
@@ -4810,11 +5051,20 @@
       <c r="AE33" s="14">
         <v>44351</v>
       </c>
-      <c r="AF33" s="13">
+      <c r="AF33" s="14">
         <v>43997</v>
       </c>
-    </row>
-    <row r="34" spans="1:32">
+      <c r="AG33" s="14">
+        <v>44288</v>
+      </c>
+      <c r="AH33" s="14">
+        <v>43511</v>
+      </c>
+      <c r="AI33" s="14"/>
+      <c r="AJ33" s="14"/>
+      <c r="AK33" s="14"/>
+    </row>
+    <row r="34" spans="1:37">
       <c r="B34" s="2" t="s">
         <v>117</v>
       </c>
@@ -4908,8 +5158,14 @@
       <c r="AF34" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="36" spans="1:32">
+      <c r="AG34" t="s">
+        <v>488</v>
+      </c>
+      <c r="AH34" s="5" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="36" spans="1:37">
       <c r="B36" t="s">
         <v>476</v>
       </c>
@@ -4917,7 +5173,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:32" ht="126" customHeight="1">
+    <row r="37" spans="1:37" ht="126" customHeight="1">
       <c r="B37" s="2" t="s">
         <v>273</v>
       </c>
@@ -4954,8 +5210,11 @@
       <c r="AF37" s="2" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="38" spans="1:32" ht="75">
+      <c r="AG37" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="38" spans="1:37" ht="72">
       <c r="B38" s="2" t="s">
         <v>233</v>
       </c>
@@ -5015,20 +5274,20 @@
         <v>435</v>
       </c>
     </row>
-    <row r="40" spans="1:32">
+    <row r="40" spans="1:37">
       <c r="D40" s="9"/>
     </row>
-    <row r="41" spans="1:32">
+    <row r="41" spans="1:37">
       <c r="B41" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:32">
+    <row r="42" spans="1:37">
       <c r="B42" s="11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:32">
+    <row r="43" spans="1:37">
       <c r="A43" s="2">
         <v>1</v>
       </c>
@@ -5047,8 +5306,14 @@
       <c r="AF43" s="16" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="44" spans="1:32">
+      <c r="AG43" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="AH43" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="44" spans="1:37">
       <c r="A44" s="2">
         <v>2</v>
       </c>
@@ -5076,8 +5341,11 @@
       <c r="AF44" s="16" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="45" spans="1:32">
+      <c r="AH44" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="45" spans="1:37">
       <c r="A45" s="2">
         <v>3</v>
       </c>
@@ -5100,7 +5368,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="46" spans="1:32">
+    <row r="46" spans="1:37">
       <c r="A46" s="2">
         <v>4</v>
       </c>
@@ -5117,7 +5385,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="47" spans="1:32">
+    <row r="47" spans="1:37">
       <c r="A47" s="2">
         <v>5</v>
       </c>
@@ -5131,7 +5399,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="48" spans="1:32">
+    <row r="48" spans="1:37">
       <c r="A48" s="2">
         <v>6</v>
       </c>
@@ -5171,8 +5439,14 @@
       <c r="AF48" s="2" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="49" spans="1:32" ht="30">
+      <c r="AG48" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="AH48" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="49" spans="1:34">
       <c r="A49" s="2">
         <v>7</v>
       </c>
@@ -5189,7 +5463,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="50" spans="1:32">
+    <row r="50" spans="1:34">
       <c r="A50" s="2">
         <v>8</v>
       </c>
@@ -5200,7 +5474,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:32">
+    <row r="51" spans="1:34">
       <c r="E51" s="2" t="s">
         <v>126</v>
       </c>
@@ -5232,7 +5506,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="52" spans="1:32" ht="30">
+    <row r="52" spans="1:34" ht="28.8">
       <c r="E52" s="2" t="s">
         <v>395</v>
       </c>
@@ -5243,7 +5517,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="53" spans="1:32" ht="30">
+    <row r="53" spans="1:34">
       <c r="E53" s="2" t="s">
         <v>129</v>
       </c>
@@ -5254,17 +5528,17 @@
         <v>479</v>
       </c>
     </row>
-    <row r="54" spans="1:32">
+    <row r="54" spans="1:34">
       <c r="J54" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="1:32">
+    <row r="55" spans="1:34">
       <c r="B55" s="11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="1:32" ht="30">
+    <row r="56" spans="1:34" ht="28.8">
       <c r="A56" s="2">
         <v>9</v>
       </c>
@@ -5319,8 +5593,14 @@
       <c r="AF56" s="2" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="57" spans="1:32">
+      <c r="AG56" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="AH56" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="57" spans="1:34">
       <c r="A57" s="2">
         <v>10</v>
       </c>
@@ -5331,7 +5611,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:32">
+    <row r="58" spans="1:34">
       <c r="A58" s="2">
         <v>11</v>
       </c>
@@ -5342,7 +5622,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="59" spans="1:32">
+    <row r="59" spans="1:34">
       <c r="A59" s="2">
         <v>12</v>
       </c>
@@ -5353,7 +5633,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="1:32" ht="30">
+    <row r="60" spans="1:34" ht="28.8">
       <c r="A60" s="2">
         <v>13</v>
       </c>
@@ -5370,12 +5650,12 @@
         <v>198</v>
       </c>
     </row>
-    <row r="62" spans="1:32">
+    <row r="62" spans="1:34">
       <c r="B62" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:32" ht="30">
+    <row r="63" spans="1:34" ht="28.8">
       <c r="A63" s="2">
         <v>14</v>
       </c>
@@ -5389,7 +5669,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="64" spans="1:32">
+    <row r="64" spans="1:34">
       <c r="A64" s="2">
         <v>15</v>
       </c>
@@ -5403,7 +5683,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="65" spans="1:32" ht="30">
+    <row r="65" spans="1:33" ht="28.8">
       <c r="A65" s="2">
         <v>16</v>
       </c>
@@ -5417,7 +5697,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="66" spans="1:32" ht="30">
+    <row r="66" spans="1:33" ht="28.8">
       <c r="A66" s="2">
         <v>17</v>
       </c>
@@ -5428,7 +5708,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="67" spans="1:32">
+    <row r="67" spans="1:33">
       <c r="A67" s="2">
         <v>18</v>
       </c>
@@ -5439,7 +5719,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="68" spans="1:32" ht="30">
+    <row r="68" spans="1:33" ht="28.8">
       <c r="A68" s="2">
         <v>19</v>
       </c>
@@ -5453,7 +5733,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="69" spans="1:32">
+    <row r="69" spans="1:33">
       <c r="A69" s="2">
         <v>20</v>
       </c>
@@ -5467,7 +5747,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="70" spans="1:32" ht="30">
+    <row r="70" spans="1:33" ht="28.8">
       <c r="A70" s="2">
         <v>21</v>
       </c>
@@ -5481,7 +5761,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="71" spans="1:32">
+    <row r="71" spans="1:33">
       <c r="A71" s="2">
         <v>22</v>
       </c>
@@ -5492,17 +5772,17 @@
         <v>103</v>
       </c>
     </row>
-    <row r="72" spans="1:32">
+    <row r="72" spans="1:33">
       <c r="J72" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="74" spans="1:32">
+    <row r="74" spans="1:33">
       <c r="B74" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="75" spans="1:32">
+    <row r="75" spans="1:33">
       <c r="A75" s="2">
         <v>23</v>
       </c>
@@ -5537,7 +5817,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="76" spans="1:32">
+    <row r="76" spans="1:33">
       <c r="A76" s="2">
         <v>24</v>
       </c>
@@ -5548,7 +5828,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="77" spans="1:32">
+    <row r="77" spans="1:33">
       <c r="A77" s="2">
         <v>25</v>
       </c>
@@ -5559,7 +5839,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="78" spans="1:32">
+    <row r="78" spans="1:33">
       <c r="A78" s="2">
         <v>26</v>
       </c>
@@ -5596,8 +5876,11 @@
       <c r="AF78" s="2" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="79" spans="1:32">
+      <c r="AG78" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="79" spans="1:33">
       <c r="A79" s="2">
         <v>27</v>
       </c>
@@ -5608,7 +5891,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="80" spans="1:32">
+    <row r="80" spans="1:33">
       <c r="A80" s="2">
         <v>28</v>
       </c>
@@ -5619,7 +5902,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="81" spans="1:32" ht="18" customHeight="1">
+    <row r="81" spans="1:34" ht="18" customHeight="1">
       <c r="A81" s="2">
         <v>29</v>
       </c>
@@ -5644,8 +5927,14 @@
       <c r="AF81" s="2" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="82" spans="1:32" ht="16.5" customHeight="1">
+      <c r="AG81" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="AH81" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="82" spans="1:34" ht="16.5" customHeight="1">
       <c r="A82" s="2">
         <v>30</v>
       </c>
@@ -5670,8 +5959,14 @@
       <c r="AF82" s="2" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="83" spans="1:32">
+      <c r="AG82" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="AH82" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="83" spans="1:34">
       <c r="A83" s="2">
         <v>31</v>
       </c>
@@ -5691,7 +5986,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="84" spans="1:32">
+    <row r="84" spans="1:34">
       <c r="A84" s="2">
         <v>32</v>
       </c>
@@ -5702,7 +5997,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="85" spans="1:32">
+    <row r="85" spans="1:34">
       <c r="A85" s="2">
         <v>33</v>
       </c>
@@ -5713,7 +6008,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="86" spans="1:32" ht="30">
+    <row r="86" spans="1:34">
       <c r="A86" s="2">
         <v>34</v>
       </c>
@@ -5800,8 +6095,13 @@
     <hyperlink ref="AC26" r:id="rId72"/>
     <hyperlink ref="AD27" r:id="rId73"/>
     <hyperlink ref="AD28" r:id="rId74"/>
+    <hyperlink ref="AG25" r:id="rId75"/>
+    <hyperlink ref="AG27" r:id="rId76"/>
+    <hyperlink ref="AG28" r:id="rId77"/>
+    <hyperlink ref="AH25" r:id="rId78"/>
+    <hyperlink ref="AH28" r:id="rId79"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId75"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId80"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add brinton + StatMeasures scripts and update table
</commit_message>
<xml_diff>
--- a/Data quality revision R overview v01.xlsx
+++ b/Data quality revision R overview v01.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="701">
   <si>
     <t>Acronym (falls vorhanden)</t>
   </si>
@@ -1699,15 +1699,569 @@
   <si>
     <t>http://georges.biomatix.org/dartR</t>
   </si>
+  <si>
+    <t>skimr</t>
+  </si>
+  <si>
+    <t>2.1.3</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=skimr</t>
+  </si>
+  <si>
+    <t>https://github.com/ropensci/skimr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skimr provides a frictionless approach to summary statistics which conforms to the principle of least surprise, displaying summary statistics the user can skim quickly to understand their data. It handles different data types and returns a skim_df object which can be included in a pipeline or displayed nicely for the human reader. Provides: 
+    - larger set of statistics than summary(), including missing, complete, n, and sd.
+    - reports each data types separately
+    - handles dates, logicals, and a variety of other types
+    - supports spark-bar and spark-line based on the pillar package.
+</t>
+  </si>
+  <si>
+    <t>R objects, R Markdown (manually through knitr)</t>
+  </si>
+  <si>
+    <t>Number of rows</t>
+  </si>
+  <si>
+    <t>whitespace, empty</t>
+  </si>
+  <si>
+    <t>uniques</t>
+  </si>
+  <si>
+    <t>Production of spark graphs for numeric data. Integration with dplyr, pipes, tidyverse and knittr. Users can specify their own statistics and classes.</t>
+  </si>
+  <si>
+    <t>https://docs.ropensci.org/skimr/</t>
+  </si>
+  <si>
+    <t>mean, sd, percentiles, histogram, min, max, median, sd, frequency, count</t>
+  </si>
+  <si>
+    <t>ordered</t>
+  </si>
+  <si>
+    <t>correlationfunnel</t>
+  </si>
+  <si>
+    <t>≥ 3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The correlationfunnel package includes a streamlined 3-step process for preparing data and performing visual Correlation Analysis. The visualization produced uncovers insights by elevating high-correlation features and loweribng low-correlation features. The shape looks like a funnel (hence the name “Correlation Funnel”), making it very efficient to understand which features are most likely to provide business insights and lend well to a machine learning model. The Correlation Funnel process uses 3 functions:
+    Transform the data into a binary format with binarize() - This step prepares semi-processed data for an optimal format (binary) for correlation analysis
+    Perform correlation analysis using correlate() - This step correlates the “binarized” data (binary features) with the target
+    Visualize the feature-target relationships using plot_correlation_funnel() - This step produces the visualization from which we can get business insights
+</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=correlationfunnel</t>
+  </si>
+  <si>
+    <t>https://github.com/business-science/correlationfunnel</t>
+  </si>
+  <si>
+    <t>0.2.0</t>
+  </si>
+  <si>
+    <t>https://business-science.github.io/correlationfunnel/</t>
+  </si>
+  <si>
+    <t>Interactive plots</t>
+  </si>
+  <si>
+    <t>correlation analysis</t>
+  </si>
+  <si>
+    <t>Correlation funnel plot</t>
+  </si>
+  <si>
+    <t>Highlights of interest</t>
+  </si>
+  <si>
+    <t>Aesthetics and functions</t>
+  </si>
+  <si>
+    <t>Tierney, N. J., &amp; Cook, D. H. (2018). Expanding tidy data principles to facilitate missing data exploration, visualization and assessment of imputations. arXiv preprint arXiv:1809.02264.</t>
+  </si>
+  <si>
+    <t>Different visualizations for relationships in missing values. Tidy framework for missings</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=naniar</t>
+  </si>
+  <si>
+    <t>https://naniar.njtierney.com/</t>
+  </si>
+  <si>
+    <t>naniar' provides data structures and functions that facilitate the plotting of missing values and examination of imputations. This allows missing data dependencies to be explored with minimal deviation from the common work patterns of 'ggplot2' and tidy data. Provides:
+1. Shadow matrices, a tidy data structure for missing data
+2. Shorthand summaries for missing data
+3. Statistical tests of missingness
+4. Visualizations for missing data</t>
+  </si>
+  <si>
+    <t>https://github.com/njtierney/naniar</t>
+  </si>
+  <si>
+    <t>https://naniar.njtierney.com/articles/naniar-visualisation.html</t>
+  </si>
+  <si>
+    <t>0.6.1</t>
+  </si>
+  <si>
+    <t>naniar (formerly named ggmissing)</t>
+  </si>
+  <si>
+    <t>only for missings</t>
+  </si>
+  <si>
+    <t>Parallel coordinate plot, decision tree, upsetr integration. Missingness along a repeating span.</t>
+  </si>
+  <si>
+    <t>TO DO: generate SHIP report - To exclude? Focus only on correlation analysis</t>
+  </si>
+  <si>
+    <t>TO DO: generate SHIP report - To exclude? Focus only on missing values (Nas)</t>
+  </si>
+  <si>
+    <t>Tool46</t>
+  </si>
+  <si>
+    <t>Tool47</t>
+  </si>
+  <si>
+    <t>Tool48</t>
+  </si>
+  <si>
+    <t>Tool49</t>
+  </si>
+  <si>
+    <t>Tool50</t>
+  </si>
+  <si>
+    <t>Jake R Conway, Alexander Lex, Nils Gehlenborg UpSetR: An R Package for the Visualization of Intersecting Sets and their Properties doi: https://doi.org/10.1093/bioinformatics/btx364</t>
+  </si>
+  <si>
+    <t>Alexander Lex, Nils Gehlenborg, Hendrik Strobelt, Romain Vuillemot, Hanspeter Pfister,
+UpSet: Visualization of Intersecting Sets,
+IEEE Transactions on Visualization and Computer Graphics (InfoVis '14), vol. 20, no. 12, pp. 1983–1992, 2014.
+doi: https://doi.org/10.1109/TVCG.2014.2346248</t>
+  </si>
+  <si>
+    <t>UpSetR</t>
+  </si>
+  <si>
+    <t>UpSetR generates static UpSet plots. The UpSet technique visualizes set intersections in a matrix layout and introduces aggregates based on groupings and queries. The matrix layout enables the effective representation of associated data, such as the number of elements in the aggregates and intersections, as well as additional summary statistics derived from subset or element attributes.</t>
+  </si>
+  <si>
+    <t>≥ 3.0</t>
+  </si>
+  <si>
+    <t>yes, shiny app</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=UpSetR</t>
+  </si>
+  <si>
+    <t>https://github.com/hms-dbmi/UpSetR</t>
+  </si>
+  <si>
+    <t>https://gehlenborglab.shinyapps.io/upsetr/</t>
+  </si>
+  <si>
+    <t>http://gehlenborglab.org/research/projects/upsetr/</t>
+  </si>
+  <si>
+    <t>1.4.0</t>
+  </si>
+  <si>
+    <t>Upset plots for  intersecting sets</t>
+  </si>
+  <si>
+    <t>To exclude: focus only on UpSet Plots</t>
+  </si>
+  <si>
+    <t>Ggally</t>
+  </si>
+  <si>
+    <t>'GGally' extends 'ggplot2' by adding several functions to reduce the complexity of combining geometric objects with transformed data. Some of these functions include a pairwise plot matrix, a two group pairwise plot matrix, a parallel coordinates plot, a survival plot, and several functions to plot networks.</t>
+  </si>
+  <si>
+    <t>2.1.2</t>
+  </si>
+  <si>
+    <t>GPL-2 | GPL-3 [expanded from: GPL (≥ 2.0)]</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=GGally</t>
+  </si>
+  <si>
+    <t>https://ggobi.github.io/ggally/</t>
+  </si>
+  <si>
+    <t>https://github.com/ggobi/ggally/</t>
+  </si>
+  <si>
+    <t>To exclude: plotting library</t>
+  </si>
+  <si>
+    <t>See different types of plots</t>
+  </si>
+  <si>
+    <t>StatMeasures</t>
+  </si>
+  <si>
+    <t>≥ 3.1.3</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=StatMeasures</t>
+  </si>
+  <si>
+    <t>Offers useful functions to perform day-to-day data manipulation operations, data quality checks and post modelling statistical checks. One can effortlessly change class of a number of variables to factor, remove duplicate observations from the data, create deciles of a variable, perform data quality checks for continuous (integer or numeric), categorical (factor) and date variables, and compute goodness of fit measures such as auc for statistical models. The functions are consistent for objects of class 'data.frame' and 'data.table', which is an enhanced 'data.frame' implemented in the package 'data.table'.</t>
+  </si>
+  <si>
+    <t>https://github.com/cran/StatMeasures</t>
+  </si>
+  <si>
+    <t>Distinct values</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>outliers</t>
+  </si>
+  <si>
+    <t>Deciles, min, max, sd, variance, percentiles, outliers, pentiles</t>
+  </si>
+  <si>
+    <t>Confusion matrix and overall accuracy of predicted binary response, Comparison of actual and predicted linear response, Area under curve of predicted binary response, Gini coefficient of a distribution, Impute missing values in a variable, Information value of an independent variable in predicting a binary
+response,  Kolmogorov-Smirnov statistic for predicted binary response, randomise rows, remove duplicates, Split modeling data into test and train set</t>
+  </si>
+  <si>
+    <t>brinton</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=brinton</t>
+  </si>
+  <si>
+    <t>https://github.com/sciencegraph/brinton</t>
+  </si>
+  <si>
+    <t>https://sciencegraph.github.io/brinton/</t>
+  </si>
+  <si>
+    <t>0.2.5</t>
+  </si>
+  <si>
+    <t>An automated graphical exploratory data analysis (EDA) tool that introduces: a.) wideplot() graphics for exploring the structure of a dataset through a grid of variables and graphic types. b.) longplot() graphics, which present the entire catalog of available graphics for representing a particular variable using a grid of graphic types and variations on these types. c.) plotup() function, which presents a particular graphic for a specific variable of a dataset. The plotup() function also makes it possible to obtain the code used to generate the graphic, meaning that the user can adjust its properties as needed.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Millán-Martínez, P., &amp; Oller, R. (2021). A Graphical EDA Tool with ggplot2: brinton. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The R Journal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(2), 311-320. https://doi.org/10.32614/RJ-2021-018</t>
+    </r>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>histograms, density, count, scatter, violin, parallel, sequence, qq plots, heatmap, boxplot, path and point-to-point graphs, scatter plot with marginal rugs</t>
+  </si>
+  <si>
+    <t>Export one particular plot (in html) or to print the ggplot2 function to produce plot in the console</t>
+  </si>
+  <si>
+    <t>cleanEHR</t>
+  </si>
+  <si>
+    <t>Excluded: Archived on 2020-02-19</t>
+  </si>
+  <si>
+    <t>Longitudinal data plots</t>
+  </si>
+  <si>
+    <t>https://github.com/ropensci/cleanEHR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An electronic health care record (EHR) data cleaning and processing platform. It focus on heterogeneous high resolution longitudinal data. It works with Critical Care Health Informatics Collaborative (CCHIC) dataset. It is created to address various data reliability and accessibility problems of EHRs as such. </t>
+  </si>
+  <si>
+    <t>Shi, S., Pérez-Suárez, D., Harris, S., MacCallum, N., Brealey, D., Singer, M., &amp; Hetherington, J. (2017). Critical care data processing tools. Journal of Open Source Software, 2(20), 513. https://joss.theoj.org/papers/10.21105/joss.00513.pdf</t>
+  </si>
+  <si>
+    <t>yes, manual</t>
+  </si>
+  <si>
+    <t>yes (yaml)</t>
+  </si>
+  <si>
+    <t>Numerical range filter</t>
+  </si>
+  <si>
+    <t>Categorical data filter</t>
+  </si>
+  <si>
+    <t>No data</t>
+  </si>
+  <si>
+    <t>yes, as filters</t>
+  </si>
+  <si>
+    <t>Imputation</t>
+  </si>
+  <si>
+    <t>https://docs.ropensci.org/cleanEHR</t>
+  </si>
+  <si>
+    <t>Data type</t>
+  </si>
+  <si>
+    <t>chipPCR: an R package to pre-process raw data of amplification curves. Rödiger S, Burdukiewicz M, Schierack P. Bioinformatics. 2015 Sep 1;31(17):2900-2. doi: 10.1093/bioinformatics/btv205. Epub 2015 Apr 24. PMID: 25913204</t>
+  </si>
+  <si>
+    <t>chipPCR</t>
+  </si>
+  <si>
+    <t>A collection of functions to pre-process amplification curve data from polymerase chain reaction (PCR) or isothermal amplification reactions. Contains functions to normalize and baseline amplification curves, to detect both the start and end of an amplification reaction, several smoothers (e.g., LOWESS, moving average, cubic splines, Savitzky-Golay), a function to detect false positive amplification reactions and a function to determine the amplification efficiency. Quantification point (Cq) methods include the first (FDM) and second approximate derivative maximum (SDM) methods (calculated by a 5-point-stencil) and the cycle threshold method. Data sets of experimental nucleic acid amplification systems ('VideoScan HCU', capillary convective PCR (ccPCR)) and commercial systems are included. Amplification curves were generated by helicase dependent amplification (HDA), ccPCR or PCR. As detection system intercalating dyes (EvaGreen, SYBR Green) and hydrolysis probes (TaqMan) were used.</t>
+  </si>
+  <si>
+    <t>1.0-2</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=chipPCR</t>
+  </si>
+  <si>
+    <t>https://github.com/michbur/chipPCR</t>
+  </si>
+  <si>
+    <t>https://pcruniversum.github.io/chipPCR/</t>
+  </si>
+  <si>
+    <t>Excluded: focus on PCR data</t>
+  </si>
+  <si>
+    <t>yes?</t>
+  </si>
+  <si>
+    <t>Malkusch, S, Hahnefeld, L, Gurke, R, Lötsch, J. Visually guided preprocessing of bioanalytical laboratory data using an interactive R notebook (pguIMP). CPT Pharmacometrics Syst Pharmacol. 2021; 10: 1371– 1381. https://doi.org/10.1002/psp4.12704</t>
+  </si>
+  <si>
+    <t>pguIMP</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=pguIMP</t>
+  </si>
+  <si>
+    <t>0.0.0.3</t>
+  </si>
+  <si>
+    <t>GPL (≥ 3)</t>
+  </si>
+  <si>
+    <t>https://github.com/SMLMS/pguIMP</t>
+  </si>
+  <si>
+    <t>In collaboration between data scientists and experts in bioanalytical diagnostics, a graphical software package for data preprocessing called pguIMP is proposed, which contains a fixed sequence of preprocessing steps to enable reproducible interactive data preprocessing. As an R-based package, it also allows direct integration into this data science environment without requiring any programming knowledge. The implementation of contemporary data processing methods, including machine-learning-based imputation techniques, ensures the generation of corrected and cleaned bioanalytical data sets that preserve data structures such as clusters better than is possible with classical methods. This was evaluated on bioanalytical data sets from lipidomics and drug research using k-nearest-neighbors-based imputation followed by k-means clustering and density-based spatial clustering of applications with noise. The R package provides a Shiny-based web interface designed to be easy to use for non–data analysis experts. It is demonstrated that the spectrum of methods provided is suitable as a standard pipeline for preprocessing bioanalytical data in biomedical research domains.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central value (median, mode), </t>
+  </si>
+  <si>
+    <t>pairwise correlation</t>
+  </si>
+  <si>
+    <t>Empirical vs theoretical distributions</t>
+  </si>
+  <si>
+    <t>log Likelihood, imputation, data normalization, pairwise robust regression</t>
+  </si>
+  <si>
+    <t>R objects, xls, odf, R markdown, latex</t>
+  </si>
+  <si>
+    <t>To do: package installation error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checkmate </t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=checkmate</t>
+  </si>
+  <si>
+    <t>https://github.com/mllg/checkmate</t>
+  </si>
+  <si>
+    <t>BSD_3_clause + file LICENSE</t>
+  </si>
+  <si>
+    <t>Lang, M. (2017). checkmate: fast argument checks for Defensive R programming. The R Journal. 9:1, 437-445. https://doi.org/10.32614/RJ-2017-028</t>
+  </si>
+  <si>
+    <t>Tests and assertions to perform frequent argument checks. Virtually every standard type of user error when passing arguments into function can be caught with a simple, readable line which produces an informative error message in case. A substantial part of the package was written in C to minimize any worries about execution time overhead. Fur thermore, checkmate simplifies writing unit tests using the framework testthat (Wickham, 2011) by extending it with plenty of additional expectation functions, and registered C routines are available for package developers to perform assertions on arbitrary SEXPs (internal data structure for R objects implemented as struct in C) in compiled code.</t>
+  </si>
+  <si>
+    <t>Excluded: focus on argument checks / unit testing</t>
+  </si>
+  <si>
+    <t>assertthat</t>
+  </si>
+  <si>
+    <t>https://github.com/hadley/assertthat</t>
+  </si>
+  <si>
+    <t>An extension to stopifnot() that makes it easy to declare the pre and post conditions that you code should satisfy, while also producing friendly error messages so that your users know what's gone wrong.</t>
+  </si>
+  <si>
+    <t>0.2.1</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=assertthat</t>
+  </si>
+  <si>
+    <t>ensurer</t>
+  </si>
+  <si>
+    <t>ensurer is a utility package for R that provides a simple and light-weight mechanism for ensuring certain aspects of values at runtime. Using the magrittr pipe %&gt;% greatly improves semantics of the functionality provided by this package, but it is not necessary.
+This package is not meant as a substitute for unit testing, and great packages for this already exist, e.g. testthat by Hadley Wickham. The ensurer package is ideal for scripts or programs where runtime conditions may break the functionality, and where errors should be raised as soon and clear as possible. Although a side-effect, It is my experience that it also promotes better design decisions at outset, and helps catch coding errors early on.</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=ensurer</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/web/packages/ensurer/vignettes/ensurer.html</t>
+  </si>
+  <si>
+    <t>Excluded: focus on argument checks at runtime</t>
+  </si>
+  <si>
+    <t>tester</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=tester</t>
+  </si>
+  <si>
+    <t>https://github.com/gastonstat/tester</t>
+  </si>
+  <si>
+    <t>tester provides human readable functions to test characteristics of some common R objects. The main purpose behind tester is to help you validate objects, especially for programming and developing purposes (e.g. creating R packages)</t>
+  </si>
+  <si>
+    <t>0.1.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exposomeShiny </t>
+  </si>
+  <si>
+    <t>Xavier Escriba-Montagut, Xavier Basagaña, Martine Vrijheid, Juan R Gonzalez, Software application profile: exposomeShiny—a toolbox for exposome data analysis, International Journal of Epidemiology, 2021;, dyab220, https://doi.org/10.1093/ije/dyab220</t>
+  </si>
+  <si>
+    <t>https://github.com/isglobal-brge/exposomeShiny</t>
+  </si>
+  <si>
+    <t>https://isglobal-brge.github.io/exposome_bookdown/</t>
+  </si>
+  <si>
+    <t>Excluded: focus on exposome analysis</t>
+  </si>
+  <si>
+    <t>standalone web application implemented in R, also available as a Docker image. Different types of analyses.</t>
+  </si>
+  <si>
+    <t>v1.4</t>
+  </si>
+  <si>
+    <t>≥ 4.0.2</t>
+  </si>
+  <si>
+    <t>ExposomeShiny is a standalone web application implemented in R (front end support for Bioconductor packages). It is available as source files and can be installed in any server or computer avoiding problems with data confidentiality. It is executed in RStudio which opens a browser window with the web application. The presented implementation allows the conduct of: (i) data pre-processing: normalization and missing imputation (including limit of detection); (ii) descriptive analysis; (iii) exposome principal component analysis (PCA) and hierarchical clustering; (iv) exposome-wide association studies (ExWAS) and variable selection ExWAS; (v) omic data integration by single association and multi-omic analyses; and (vi) post-exposome data analyses to gain biological insight for the exposures, genes or using the Comparative Toxicogenomics Database (CTD) and pathway analysis.</t>
+  </si>
+  <si>
+    <t>assertr</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=assertr</t>
+  </si>
+  <si>
+    <t>https://docs.ropensci.org/assertr/</t>
+  </si>
+  <si>
+    <t>https://github.com/ropensci/assertr</t>
+  </si>
+  <si>
+    <t>The assertr package supplies a suite of functions designed to verify assumptions about data early in an analysis pipeline so that data errors are spotted early and can be addressed quickly.</t>
+  </si>
+  <si>
+    <t>within_bounds</t>
+  </si>
+  <si>
+    <t>in_set</t>
+  </si>
+  <si>
+    <t>duplicated_across_cols</t>
+  </si>
+  <si>
+    <t>has_class</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> within_n_sds - used to dynamically create bounds to check vector elements with based on standard z-scores
+ within_n_mads - better method for dynamically creating bounds to check vector elements with based on 'robust' z-scores (using median absolute deviation)
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1760,6 +2314,12 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1794,7 +2354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1841,6 +2401,26 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -2122,13 +2702,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV86"/>
+  <dimension ref="A1:BA87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="AJ3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="AZ12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AK6" sqref="AK6"/>
+      <selection pane="bottomRight" activeCell="BA18" sqref="BA18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4"/>
@@ -2169,10 +2749,25 @@
     <col min="35" max="35" width="28.44140625" style="2" customWidth="1"/>
     <col min="36" max="36" width="24.109375" style="2" customWidth="1"/>
     <col min="37" max="37" width="22.77734375" style="2" customWidth="1"/>
-    <col min="38" max="16384" width="11" style="2"/>
+    <col min="38" max="38" width="24" style="2" customWidth="1"/>
+    <col min="39" max="39" width="26.5546875" style="2" customWidth="1"/>
+    <col min="40" max="40" width="26.6640625" style="2" customWidth="1"/>
+    <col min="41" max="41" width="27.77734375" style="2" customWidth="1"/>
+    <col min="42" max="42" width="24.33203125" style="2" customWidth="1"/>
+    <col min="43" max="43" width="31.5546875" style="2" customWidth="1"/>
+    <col min="44" max="44" width="26" style="2" customWidth="1"/>
+    <col min="45" max="45" width="26.109375" style="2" customWidth="1"/>
+    <col min="46" max="46" width="25.6640625" style="2" customWidth="1"/>
+    <col min="47" max="47" width="29.44140625" style="2" customWidth="1"/>
+    <col min="48" max="48" width="29.5546875" style="2" customWidth="1"/>
+    <col min="49" max="49" width="26.88671875" style="2" customWidth="1"/>
+    <col min="50" max="50" width="25.6640625" style="2" customWidth="1"/>
+    <col min="51" max="52" width="28.33203125" style="2" customWidth="1"/>
+    <col min="53" max="53" width="25.21875" style="2" customWidth="1"/>
+    <col min="54" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:48" s="4" customFormat="1">
+    <row r="1" spans="2:53" s="4" customFormat="1">
       <c r="B1" s="4" t="s">
         <v>18</v>
       </c>
@@ -2314,8 +2909,23 @@
       <c r="AV1" s="4" t="s">
         <v>390</v>
       </c>
+      <c r="AW1" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="AX1" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="AY1" s="4" t="s">
+        <v>578</v>
+      </c>
+      <c r="AZ1" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="BA1" s="4" t="s">
+        <v>580</v>
+      </c>
     </row>
-    <row r="2" spans="2:48">
+    <row r="2" spans="2:53" ht="28.8">
       <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
@@ -2424,8 +3034,56 @@
       <c r="AK2" s="2" t="s">
         <v>529</v>
       </c>
+      <c r="AL2" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="BA2" s="2" t="s">
+        <v>691</v>
+      </c>
     </row>
-    <row r="3" spans="2:48">
+    <row r="3" spans="2:53">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2534,8 +3192,56 @@
       <c r="AK3" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="AL3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AR3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AS3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AV3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AX3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AY3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AZ3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="BA3" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="2:48">
+    <row r="4" spans="2:53">
       <c r="B4" s="2" t="s">
         <v>49</v>
       </c>
@@ -2644,8 +3350,56 @@
       <c r="AK4" s="2" t="s">
         <v>530</v>
       </c>
+      <c r="AL4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>552</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>585</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>552</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>604</v>
+      </c>
+      <c r="AR4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>200</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>367</v>
+      </c>
+      <c r="AU4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>367</v>
+      </c>
+      <c r="AW4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AX4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AY4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>689</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>200</v>
+      </c>
     </row>
-    <row r="5" spans="2:48">
+    <row r="5" spans="2:53">
       <c r="B5" s="8" t="s">
         <v>77</v>
       </c>
@@ -2754,8 +3508,53 @@
       <c r="AK5" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="AL5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AN5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AQ5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AU5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AV5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AW5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AY5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="BA5" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="6" spans="2:48">
+    <row r="6" spans="2:53">
       <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
@@ -2864,8 +3663,56 @@
       <c r="AK6" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="AL6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO6" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="AP6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT6" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="AU6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AV6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AW6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AX6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AY6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AZ6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="BA6" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="7" spans="2:48" ht="28.8">
+    <row r="7" spans="2:53" ht="28.8">
       <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
@@ -2974,8 +3821,53 @@
       <c r="AK7" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="AL7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AU7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AV7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AW7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AX7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AY7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="BA7" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="8" spans="2:48" ht="28.8">
+    <row r="8" spans="2:53" ht="28.8">
       <c r="B8" s="2" t="s">
         <v>40</v>
       </c>
@@ -3081,8 +3973,50 @@
       <c r="AK8" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="AL8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AV8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AW8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AX8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AY8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="BA8" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="9" spans="2:48" ht="246" customHeight="1">
+    <row r="9" spans="2:53" ht="246" customHeight="1">
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
@@ -3191,12 +4125,56 @@
       <c r="AK9" s="7" t="s">
         <v>535</v>
       </c>
-      <c r="AL9" s="7"/>
-      <c r="AM9" s="7"/>
-      <c r="AN9" s="7"/>
-      <c r="AO9" s="7"/>
+      <c r="AL9" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="AM9" s="7" t="s">
+        <v>553</v>
+      </c>
+      <c r="AN9" s="21" t="s">
+        <v>567</v>
+      </c>
+      <c r="AO9" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="AP9" s="7" t="s">
+        <v>595</v>
+      </c>
+      <c r="AQ9" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="AR9" s="7" t="s">
+        <v>618</v>
+      </c>
+      <c r="AS9" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="AT9" s="7" t="s">
+        <v>640</v>
+      </c>
+      <c r="AU9" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="AV9" s="7" t="s">
+        <v>665</v>
+      </c>
+      <c r="AW9" s="7" t="s">
+        <v>669</v>
+      </c>
+      <c r="AX9" s="7" t="s">
+        <v>673</v>
+      </c>
+      <c r="AY9" s="7" t="s">
+        <v>680</v>
+      </c>
+      <c r="AZ9" s="7" t="s">
+        <v>690</v>
+      </c>
+      <c r="BA9" s="7" t="s">
+        <v>695</v>
+      </c>
     </row>
-    <row r="10" spans="2:48">
+    <row r="10" spans="2:53">
       <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
@@ -3305,8 +4283,56 @@
       <c r="AK10" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="AL10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AU10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AV10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AX10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AY10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AZ10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="BA10" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="11" spans="2:48" ht="28.8">
+    <row r="11" spans="2:53" ht="28.8">
       <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
@@ -3415,8 +4441,56 @@
       <c r="AK11" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="AL11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AU11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AV11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AX11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AY11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AZ11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="BA11" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="12" spans="2:48" ht="115.2">
+    <row r="12" spans="2:53" ht="115.2">
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
@@ -3525,8 +4599,56 @@
       <c r="AK12" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="AL12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AU12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AV12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AX12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AY12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AZ12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="BA12" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="13" spans="2:48" ht="29.25" customHeight="1">
+    <row r="13" spans="2:53" ht="29.25" customHeight="1">
       <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
@@ -3608,8 +4730,33 @@
       <c r="AI13" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="AL13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AN13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AU13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="BA13"/>
     </row>
-    <row r="14" spans="2:48" ht="28.8">
+    <row r="14" spans="2:53" ht="28.8">
       <c r="B14" s="2" t="s">
         <v>45</v>
       </c>
@@ -3694,8 +4841,32 @@
       <c r="AI14" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="AL14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AN14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AU14" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="15" spans="2:48" ht="28.8">
+    <row r="15" spans="2:53" ht="28.8">
       <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
@@ -3780,8 +4951,32 @@
       <c r="AI15" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="AL15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AU15" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="16" spans="2:48" ht="27.6" customHeight="1">
+    <row r="16" spans="2:53" ht="27.6" customHeight="1">
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
@@ -3866,8 +5061,35 @@
       <c r="AI16" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="AL16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AN16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AU16" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="17" spans="2:37" ht="151.19999999999999" customHeight="1">
+    <row r="17" spans="2:53" ht="151.19999999999999" customHeight="1">
       <c r="B17" s="2" t="s">
         <v>44</v>
       </c>
@@ -3952,8 +5174,29 @@
       <c r="AJ17" s="7" t="s">
         <v>526</v>
       </c>
+      <c r="AL17" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="AM17" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="AN17" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="AQ17" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="AS17" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="AU17" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="BA17" s="2" t="s">
+        <v>700</v>
+      </c>
     </row>
-    <row r="18" spans="2:37" ht="28.8">
+    <row r="18" spans="2:53" ht="28.8">
       <c r="B18" s="2" t="s">
         <v>27</v>
       </c>
@@ -4056,8 +5299,47 @@
       <c r="AK18" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="AL18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS18" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="AU18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AV18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AW18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AX18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AY18" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="19" spans="2:37" ht="28.8">
+    <row r="19" spans="2:53" ht="28.8">
       <c r="B19" s="2" t="s">
         <v>28</v>
       </c>
@@ -4160,8 +5442,47 @@
       <c r="AK19" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="AL19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS19" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="AU19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AV19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AW19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AX19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AY19" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="20" spans="2:37" ht="28.8">
+    <row r="20" spans="2:53" ht="28.8">
       <c r="B20" s="2" t="s">
         <v>29</v>
       </c>
@@ -4264,8 +5585,47 @@
       <c r="AK20" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="AL20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AU20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AV20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AW20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AX20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AY20" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="21" spans="2:37" ht="28.8">
+    <row r="21" spans="2:53" ht="28.8">
       <c r="B21" s="2" t="s">
         <v>30</v>
       </c>
@@ -4374,8 +5734,38 @@
       <c r="AK21" s="2" t="s">
         <v>236</v>
       </c>
+      <c r="AL21" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="AM21" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="AN21" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="AO21" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="AP21" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="AQ21" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="AR21" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="AS21" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="AU21" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="BA21" s="2" t="s">
+        <v>236</v>
+      </c>
     </row>
-    <row r="22" spans="2:37" ht="28.8">
+    <row r="22" spans="2:53" ht="28.8">
       <c r="B22" s="2" t="s">
         <v>35</v>
       </c>
@@ -4481,8 +5871,50 @@
       <c r="AK22" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="AL22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AN22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AQ22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AU22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AV22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AW22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AY22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="BA22" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="23" spans="2:37" ht="28.8">
+    <row r="23" spans="2:53" ht="28.8">
       <c r="B23" s="2" t="s">
         <v>37</v>
       </c>
@@ -4585,8 +6017,47 @@
       <c r="AJ23" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="AL23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS23" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="AU23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AV23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AX23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AY23" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="24" spans="2:37" ht="28.8">
+    <row r="24" spans="2:53" ht="28.8">
       <c r="B24" s="2" t="s">
         <v>39</v>
       </c>
@@ -4689,8 +6160,50 @@
       <c r="AJ24" s="2" t="s">
         <v>528</v>
       </c>
+      <c r="AL24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AU24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AV24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AX24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AY24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="BA24" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="25" spans="2:37" ht="90" customHeight="1">
+    <row r="25" spans="2:53" ht="90" customHeight="1">
       <c r="B25" s="2" t="s">
         <v>31</v>
       </c>
@@ -4768,8 +6281,44 @@
       <c r="AK25" s="7" t="s">
         <v>533</v>
       </c>
+      <c r="AL25" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="AM25" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="AN25" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="AO25" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="AP25" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="AQ25" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="AR25" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="AS25" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="AT25" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="AU25" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="AV25" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="AZ25" s="2" t="s">
+        <v>683</v>
+      </c>
     </row>
-    <row r="26" spans="2:37" ht="43.2">
+    <row r="26" spans="2:53" ht="43.2">
       <c r="B26" s="2" t="s">
         <v>137</v>
       </c>
@@ -4851,8 +6400,41 @@
       <c r="AK26" s="3" t="s">
         <v>532</v>
       </c>
+      <c r="AL26" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AN26" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="AO26" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="AR26" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="AT26" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="AU26" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="AV26" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="AW26" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="AX26" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="AY26" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="BA26" s="2" t="s">
+        <v>692</v>
+      </c>
     </row>
-    <row r="27" spans="2:37" ht="43.2">
+    <row r="27" spans="2:53" ht="43.2">
       <c r="B27" s="2" t="s">
         <v>3</v>
       </c>
@@ -4934,8 +6516,38 @@
       <c r="AK27" s="3" t="s">
         <v>537</v>
       </c>
+      <c r="AL27" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="AM27" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="AN27" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="AO27" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="AP27" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="AR27" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="AS27" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="AT27" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="AZ27" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="BA27" s="2" t="s">
+        <v>693</v>
+      </c>
     </row>
-    <row r="28" spans="2:37" ht="28.8">
+    <row r="28" spans="2:53" ht="28.8">
       <c r="B28" s="2" t="s">
         <v>32</v>
       </c>
@@ -5038,8 +6650,53 @@
       <c r="AK28" s="3" t="s">
         <v>536</v>
       </c>
+      <c r="AL28" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="AM28" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="AN28" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="AO28" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="AP28" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="AQ28" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="AR28" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="AS28" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="AT28" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="AU28" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="AV28" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="AW28" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="AY28" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="AZ28" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="BA28" s="2" t="s">
+        <v>694</v>
+      </c>
     </row>
-    <row r="29" spans="2:37" ht="43.2">
+    <row r="29" spans="2:53" ht="172.8">
       <c r="D29" s="3" t="s">
         <v>140</v>
       </c>
@@ -5057,11 +6714,26 @@
       <c r="AA29" s="3" t="s">
         <v>375</v>
       </c>
+      <c r="AL29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN29" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="AO29" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AX29" s="2" t="s">
+        <v>675</v>
+      </c>
     </row>
-    <row r="30" spans="2:37">
+    <row r="30" spans="2:53" ht="28.8">
       <c r="D30" s="3"/>
+      <c r="AO30" s="2" t="s">
+        <v>589</v>
+      </c>
     </row>
-    <row r="31" spans="2:37">
+    <row r="31" spans="2:53" ht="28.8">
       <c r="B31" s="2" t="s">
         <v>33</v>
       </c>
@@ -5167,8 +6839,53 @@
       <c r="AK31" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="AL31" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM31" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="AN31" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="AO31" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="AP31" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="AQ31" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AR31" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS31" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT31" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU31" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="AV31" t="s">
+        <v>663</v>
+      </c>
+      <c r="AW31" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="AX31" t="s">
+        <v>231</v>
+      </c>
+      <c r="AY31" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="BA31" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="32" spans="2:37">
+    <row r="32" spans="2:53">
       <c r="B32" s="8" t="s">
         <v>78</v>
       </c>
@@ -5275,8 +6992,56 @@
       <c r="AK32" s="13">
         <v>42909</v>
       </c>
+      <c r="AL32" s="13">
+        <v>43110</v>
+      </c>
+      <c r="AM32" s="13">
+        <v>43683</v>
+      </c>
+      <c r="AN32" s="13">
+        <v>42956</v>
+      </c>
+      <c r="AO32" s="13">
+        <v>42201</v>
+      </c>
+      <c r="AP32" s="22">
+        <v>40210</v>
+      </c>
+      <c r="AQ32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR32" s="13">
+        <v>43799</v>
+      </c>
+      <c r="AS32" s="24">
+        <v>42768</v>
+      </c>
+      <c r="AT32" s="13">
+        <v>41620</v>
+      </c>
+      <c r="AU32" s="13">
+        <v>44378</v>
+      </c>
+      <c r="AV32" s="13">
+        <v>41807</v>
+      </c>
+      <c r="AW32" s="13">
+        <v>41614</v>
+      </c>
+      <c r="AX32" s="13">
+        <v>41961</v>
+      </c>
+      <c r="AY32" s="13">
+        <v>41467</v>
+      </c>
+      <c r="AZ32" s="24">
+        <v>44075</v>
+      </c>
+      <c r="BA32" s="13">
+        <v>42087</v>
+      </c>
     </row>
-    <row r="33" spans="1:37">
+    <row r="33" spans="1:53">
       <c r="B33" s="8" t="s">
         <v>118</v>
       </c>
@@ -5385,8 +7150,56 @@
       <c r="AK33" s="13">
         <v>44344</v>
       </c>
+      <c r="AL33" s="13">
+        <v>44262</v>
+      </c>
+      <c r="AM33" s="18">
+        <v>43991</v>
+      </c>
+      <c r="AN33" s="13">
+        <v>44330</v>
+      </c>
+      <c r="AO33" s="13">
+        <v>43607</v>
+      </c>
+      <c r="AP33" s="13">
+        <v>44368</v>
+      </c>
+      <c r="AQ33" s="13">
+        <v>42090</v>
+      </c>
+      <c r="AR33" s="13">
+        <v>44288</v>
+      </c>
+      <c r="AS33" s="13">
+        <v>43085</v>
+      </c>
+      <c r="AT33" s="13">
+        <v>44260</v>
+      </c>
+      <c r="AU33" s="13">
+        <v>44469</v>
+      </c>
+      <c r="AV33" s="13">
+        <v>43867</v>
+      </c>
+      <c r="AW33" s="13">
+        <v>43545</v>
+      </c>
+      <c r="AX33" s="13">
+        <v>42115</v>
+      </c>
+      <c r="AY33" s="13">
+        <v>41592</v>
+      </c>
+      <c r="AZ33" s="24">
+        <v>44257</v>
+      </c>
+      <c r="BA33" s="13">
+        <v>44221</v>
+      </c>
     </row>
-    <row r="34" spans="1:37">
+    <row r="34" spans="1:53">
       <c r="B34" s="2" t="s">
         <v>117</v>
       </c>
@@ -5495,11 +7308,62 @@
       <c r="AK34" t="s">
         <v>531</v>
       </c>
+      <c r="AL34" t="s">
+        <v>539</v>
+      </c>
+      <c r="AM34" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="AN34" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="AO34" t="s">
+        <v>591</v>
+      </c>
+      <c r="AP34" t="s">
+        <v>596</v>
+      </c>
+      <c r="AQ34" s="23">
+        <v>1</v>
+      </c>
+      <c r="AR34" t="s">
+        <v>617</v>
+      </c>
+      <c r="AS34" s="23">
+        <v>1</v>
+      </c>
+      <c r="AT34" t="s">
+        <v>641</v>
+      </c>
+      <c r="AU34" t="s">
+        <v>650</v>
+      </c>
+      <c r="AV34" t="s">
+        <v>186</v>
+      </c>
+      <c r="AW34" t="s">
+        <v>670</v>
+      </c>
+      <c r="AX34">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AY34" t="s">
+        <v>681</v>
+      </c>
+      <c r="AZ34" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="BA34">
+        <v>2.8</v>
+      </c>
     </row>
-    <row r="36" spans="1:37">
+    <row r="36" spans="1:53">
       <c r="B36" t="s">
         <v>476</v>
       </c>
+      <c r="C36" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="AF36" s="2" t="s">
         <v>13</v>
       </c>
@@ -5509,11 +7373,26 @@
       <c r="AJ36" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="AL36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AN36" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="AO36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ36" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="37" spans="1:37" ht="126" customHeight="1">
+    <row r="37" spans="1:53" ht="126" customHeight="1">
       <c r="B37" s="2" t="s">
         <v>273</v>
       </c>
+      <c r="C37" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="E37" s="5" t="s">
         <v>402</v>
       </c>
@@ -5553,8 +7432,32 @@
       <c r="AI37" s="2" t="s">
         <v>517</v>
       </c>
+      <c r="AL37" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="AN37" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO37" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ37" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="AR37" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="AU37" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="AV37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW37" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="38" spans="1:37" ht="86.4">
+    <row r="38" spans="1:53" ht="86.4">
       <c r="B38" s="2" t="s">
         <v>233</v>
       </c>
@@ -5613,704 +7516,858 @@
       <c r="AC38" s="2" t="s">
         <v>435</v>
       </c>
+      <c r="AI38" s="20" t="s">
+        <v>527</v>
+      </c>
       <c r="AJ38" s="17" t="s">
         <v>527</v>
       </c>
       <c r="AK38" s="2" t="s">
         <v>534</v>
       </c>
+      <c r="AL38" s="20" t="s">
+        <v>527</v>
+      </c>
+      <c r="AM38" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="AN38" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="AO38" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="AP38" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="AS38" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="AT38" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="AU38" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="AV38" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="AW38" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="AX38" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="AY38" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="AZ38" s="2" t="s">
+        <v>686</v>
+      </c>
     </row>
-    <row r="40" spans="1:37">
-      <c r="D40" s="9"/>
-      <c r="AJ40" s="1"/>
+    <row r="39" spans="1:53" ht="57.6">
+      <c r="B39" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" s="5"/>
+      <c r="F39" s="6"/>
+      <c r="AI39" s="20"/>
+      <c r="AJ39" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="AL39" s="20"/>
+      <c r="AM39" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="AN39" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="AO39" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="AP39" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="AR39" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="AS39" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="AZ39" s="2" t="s">
+        <v>687</v>
+      </c>
     </row>
-    <row r="41" spans="1:37">
-      <c r="B41" s="1" t="s">
+    <row r="41" spans="1:53">
+      <c r="D41" s="9"/>
+      <c r="AJ41" s="1"/>
+    </row>
+    <row r="42" spans="1:53">
+      <c r="B42" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:37">
-      <c r="B42" s="11" t="s">
+    <row r="43" spans="1:53">
+      <c r="B43" s="11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:37">
-      <c r="A43" s="2">
+    <row r="44" spans="1:53">
+      <c r="A44" s="2">
         <v>1</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="AB43" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="AF43" s="16" t="s">
-        <v>482</v>
-      </c>
-      <c r="AG43" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="AH43" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="AI43" s="2" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="44" spans="1:37">
-      <c r="A44" s="2">
-        <v>2</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="AA44" s="2" t="s">
-        <v>392</v>
-      </c>
       <c r="AB44" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="AC44" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="AD44" s="2" t="s">
-        <v>448</v>
-      </c>
       <c r="AF44" s="16" t="s">
         <v>482</v>
       </c>
+      <c r="AG44" s="2" t="s">
+        <v>492</v>
+      </c>
       <c r="AH44" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="AI44" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="AL44" s="2" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="45" spans="1:53">
+      <c r="A45" s="2">
+        <v>2</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="AA45" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="AB45" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="AC45" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="AD45" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="AF45" s="16" t="s">
+        <v>482</v>
+      </c>
+      <c r="AH45" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="AI44" s="2" t="s">
+      <c r="AI45" s="2" t="s">
         <v>515</v>
       </c>
+      <c r="AL45" s="2" t="s">
+        <v>492</v>
+      </c>
     </row>
-    <row r="45" spans="1:37">
-      <c r="A45" s="2">
+    <row r="46" spans="1:53">
+      <c r="A46" s="2">
         <v>3</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="H46" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="U45" s="2" t="s">
+      <c r="U46" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="AA45" s="2" t="s">
+      <c r="AA46" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="AI45" s="2" t="s">
+      <c r="AI46" s="2" t="s">
         <v>516</v>
       </c>
+      <c r="BA46" s="2" t="s">
+        <v>698</v>
+      </c>
     </row>
-    <row r="46" spans="1:37">
-      <c r="A46" s="2">
+    <row r="47" spans="1:53">
+      <c r="A47" s="2">
         <v>4</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="W46" s="2" t="s">
+      <c r="W47" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="AA46" s="2" t="s">
+      <c r="AA47" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="47" spans="1:37">
-      <c r="A47" s="2">
+    <row r="48" spans="1:53">
+      <c r="A48" s="2">
         <v>5</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="W47" s="2" t="s">
+      <c r="W48" s="2" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="48" spans="1:37">
-      <c r="A48" s="2">
+    <row r="49" spans="1:53">
+      <c r="A49" s="2">
         <v>6</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="H49" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="J48" s="2" t="s">
+      <c r="J49" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="W48" s="2" t="s">
+      <c r="W49" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="Z48" s="2" t="s">
+      <c r="Z49" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="AA48" s="2" t="s">
+      <c r="AA49" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="AC48" s="2" t="s">
+      <c r="AC49" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="AE48" s="2" t="s">
+      <c r="AE49" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="AF48" s="2" t="s">
+      <c r="AF49" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="AG48" s="2" t="s">
+      <c r="AG49" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="AH48" s="2" t="s">
+      <c r="AH49" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="AI48" s="2" t="s">
+      <c r="AI49" s="2" t="s">
         <v>458</v>
       </c>
+      <c r="AL49" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="AQ49" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="AS49" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="BA49" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
-    <row r="49" spans="1:35">
-      <c r="A49" s="2">
+    <row r="50" spans="1:53">
+      <c r="A50" s="2">
         <v>7</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="J49" s="2" t="s">
+      <c r="J50" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="50" spans="1:35">
-      <c r="A50" s="2">
+    <row r="51" spans="1:53">
+      <c r="A51" s="2">
         <v>8</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:35">
-      <c r="E51" s="2" t="s">
+    <row r="52" spans="1:53">
+      <c r="E52" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="H52" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J51" s="2" t="s">
+      <c r="J52" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="K51" s="2" t="s">
+      <c r="K52" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="M51" s="2" t="s">
+      <c r="M52" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="W51" s="2" t="s">
+      <c r="W52" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="Z51" s="2" t="s">
+      <c r="Z52" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="AC51" s="2" t="s">
+      <c r="AC52" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="AE51" s="2" t="s">
+      <c r="AE52" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="AF51" s="2" t="s">
+      <c r="AF52" s="2" t="s">
         <v>478</v>
       </c>
+      <c r="AL52" s="2" t="s">
+        <v>546</v>
+      </c>
     </row>
-    <row r="52" spans="1:35" ht="28.8">
-      <c r="E52" s="2" t="s">
+    <row r="53" spans="1:53" ht="28.8">
+      <c r="E53" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="J52" s="2" t="s">
+      <c r="J53" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="AF52" t="s">
+      <c r="AF53" t="s">
         <v>483</v>
       </c>
+      <c r="AL53" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="AQ53" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="AS53" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="BA53" s="2" t="s">
+        <v>478</v>
+      </c>
     </row>
-    <row r="53" spans="1:35">
-      <c r="E53" s="2" t="s">
+    <row r="54" spans="1:53">
+      <c r="E54" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="J53" s="2" t="s">
+      <c r="J54" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="AF53" s="2" t="s">
+      <c r="AF54" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="AI53" s="2" t="s">
+      <c r="AI54" s="2" t="s">
         <v>513</v>
       </c>
+      <c r="AL54" s="2" t="s">
+        <v>550</v>
+      </c>
     </row>
-    <row r="54" spans="1:35">
-      <c r="J54" s="2" t="s">
+    <row r="55" spans="1:53">
+      <c r="J55" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="1:35">
-      <c r="B55" s="11" t="s">
+    <row r="56" spans="1:53">
+      <c r="B56" s="11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="1:35" ht="28.8">
-      <c r="A56" s="2">
+    <row r="57" spans="1:53" ht="28.8">
+      <c r="A57" s="2">
         <v>9</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="E57" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="F57" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G56" s="2" t="s">
+      <c r="G57" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="H56" s="2" t="s">
+      <c r="H57" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="J56" s="2" t="s">
+      <c r="J57" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="K56" s="2" t="s">
+      <c r="K57" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="M56" s="2" t="s">
+      <c r="M57" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="V56" s="2" t="s">
+      <c r="V57" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="W56" s="2" t="s">
+      <c r="W57" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="Z56" s="2" t="s">
+      <c r="Z57" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="AA56" s="2" t="s">
+      <c r="AA57" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="AB56" s="2" t="s">
+      <c r="AB57" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="AC56" s="2" t="s">
+      <c r="AC57" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="AE56" s="2" t="s">
+      <c r="AE57" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="AF56" s="2" t="s">
+      <c r="AF57" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="AG56" s="2" t="s">
+      <c r="AG57" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="AH56" s="2" t="s">
+      <c r="AH57" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="AI56" s="2" t="s">
+      <c r="AI57" s="2" t="s">
         <v>429</v>
       </c>
+      <c r="AL57" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="AN57" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="AQ57" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="AR57" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="AS57" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="AU57" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="BA57" s="2" t="s">
+        <v>429</v>
+      </c>
     </row>
-    <row r="57" spans="1:35">
-      <c r="A57" s="2">
+    <row r="58" spans="1:53">
+      <c r="A58" s="2">
         <v>10</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:35">
-      <c r="A58" s="2">
+    <row r="59" spans="1:53">
+      <c r="A59" s="2">
         <v>11</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="59" spans="1:35">
-      <c r="A59" s="2">
+    <row r="60" spans="1:53">
+      <c r="A60" s="2">
         <v>12</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="1:35" ht="28.8">
-      <c r="A60" s="2">
-        <v>13</v>
-      </c>
-      <c r="B60" s="2" t="s">
+    <row r="61" spans="1:53" ht="28.8">
+      <c r="A61" s="2">
+        <v>13</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="K60" s="2" t="s">
+      <c r="K61" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="62" spans="1:35">
-      <c r="B62" s="11" t="s">
+    <row r="63" spans="1:53">
+      <c r="B63" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:35" ht="28.8">
-      <c r="A63" s="2">
+    <row r="64" spans="1:53" ht="28.8">
+      <c r="A64" s="2">
         <v>14</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="J63" s="2" t="s">
+      <c r="J64" s="2" t="s">
         <v>162</v>
       </c>
+      <c r="AS64" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="BA64" s="2" t="s">
+        <v>696</v>
+      </c>
     </row>
-    <row r="64" spans="1:35">
-      <c r="A64" s="2">
-        <v>15</v>
-      </c>
-      <c r="B64" s="2" t="s">
+    <row r="65" spans="1:53">
+      <c r="A65" s="2">
+        <v>15</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="J64" s="2" t="s">
+      <c r="J65" s="2" t="s">
         <v>163</v>
       </c>
+      <c r="AS65" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="BA65" s="2" t="s">
+        <v>696</v>
+      </c>
     </row>
-    <row r="65" spans="1:35" ht="28.8">
-      <c r="A65" s="2">
+    <row r="66" spans="1:53" ht="28.8">
+      <c r="A66" s="2">
         <v>16</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="J65" s="2" t="s">
+      <c r="J66" s="2" t="s">
         <v>164</v>
       </c>
+      <c r="BA66" s="2" t="s">
+        <v>697</v>
+      </c>
     </row>
-    <row r="66" spans="1:35" ht="28.8">
-      <c r="A66" s="2">
+    <row r="67" spans="1:53" ht="28.8">
+      <c r="A67" s="2">
         <v>17</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="67" spans="1:35">
-      <c r="A67" s="2">
+    <row r="68" spans="1:53">
+      <c r="A68" s="2">
         <v>18</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="68" spans="1:35" ht="28.8">
-      <c r="A68" s="2">
-        <v>19</v>
-      </c>
-      <c r="B68" s="2" t="s">
+    <row r="69" spans="1:53" ht="28.8">
+      <c r="A69" s="2">
+        <v>19</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="D69" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="J68" s="2" t="s">
+      <c r="J69" s="2" t="s">
         <v>162</v>
       </c>
+      <c r="AS69" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="BA69" s="2" t="s">
+        <v>696</v>
+      </c>
     </row>
-    <row r="69" spans="1:35">
-      <c r="A69" s="2">
+    <row r="70" spans="1:53">
+      <c r="A70" s="2">
         <v>20</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D70" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="J69" s="2" t="s">
+      <c r="J70" s="2" t="s">
         <v>163</v>
       </c>
+      <c r="BA70" s="2" t="s">
+        <v>696</v>
+      </c>
     </row>
-    <row r="70" spans="1:35" ht="28.8">
-      <c r="A70" s="2">
+    <row r="71" spans="1:53" ht="28.8">
+      <c r="A71" s="2">
         <v>21</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="J70" s="2" t="s">
+      <c r="J71" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="71" spans="1:35">
-      <c r="A71" s="2">
+    <row r="72" spans="1:53">
+      <c r="A72" s="2">
         <v>22</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="72" spans="1:35">
-      <c r="J72" s="2" t="s">
+    <row r="73" spans="1:53">
+      <c r="J73" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="74" spans="1:35">
-      <c r="B74" s="11" t="s">
+    <row r="75" spans="1:53">
+      <c r="B75" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="75" spans="1:35">
-      <c r="A75" s="2">
+    <row r="76" spans="1:53">
+      <c r="A76" s="2">
         <v>23</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D76" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="E76" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="H75" s="2" t="s">
+      <c r="H76" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="K75" s="2" t="s">
+      <c r="K76" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="W75" s="2" t="s">
+      <c r="W76" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="AC75" s="2" t="s">
+      <c r="AC76" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="AD75" t="s">
+      <c r="AD76" t="s">
         <v>449</v>
       </c>
-      <c r="AE75" s="2" t="s">
+      <c r="AE76" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="AF75" s="2" t="s">
+      <c r="AF76" s="2" t="s">
         <v>440</v>
       </c>
+      <c r="AQ76" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="AU76" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="BA76" s="2" t="s">
+        <v>610</v>
+      </c>
     </row>
-    <row r="76" spans="1:35">
-      <c r="A76" s="2">
+    <row r="77" spans="1:53">
+      <c r="A77" s="2">
         <v>24</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D77" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="77" spans="1:35">
-      <c r="A77" s="2">
+    <row r="78" spans="1:53">
+      <c r="A78" s="2">
         <v>25</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="78" spans="1:35">
-      <c r="A78" s="2">
+    <row r="79" spans="1:53" ht="28.8">
+      <c r="A79" s="2">
         <v>26</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E79" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="F79" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="H78" s="2" t="s">
+      <c r="H79" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="K78" s="2" t="s">
+      <c r="K79" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="V78" s="2" t="s">
+      <c r="V79" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="W78" s="2" t="s">
+      <c r="W79" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="AD78" s="2" t="s">
+      <c r="AD79" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="AE78" s="2" t="s">
+      <c r="AE79" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="AF78" s="2" t="s">
+      <c r="AF79" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="AG78" s="2" t="s">
+      <c r="AG79" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="AI78" s="2" t="s">
+      <c r="AI79" s="2" t="s">
         <v>414</v>
       </c>
+      <c r="AL79" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="AN79" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="AR79" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="AU79" s="2" t="s">
+        <v>656</v>
+      </c>
     </row>
-    <row r="79" spans="1:35">
-      <c r="A79" s="2">
+    <row r="80" spans="1:53">
+      <c r="A80" s="2">
         <v>27</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D80" s="2" t="s">
         <v>109</v>
       </c>
+      <c r="AL80" s="2" t="s">
+        <v>414</v>
+      </c>
     </row>
-    <row r="80" spans="1:35">
-      <c r="A80" s="2">
+    <row r="81" spans="1:47">
+      <c r="A81" s="2">
         <v>28</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="D81" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="81" spans="1:34" ht="18" customHeight="1">
-      <c r="A81" s="2">
+    <row r="82" spans="1:47" ht="18" customHeight="1">
+      <c r="A82" s="2">
         <v>29</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D81" s="2" t="s">
+      <c r="D82" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="H81" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="V81" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="AD81" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="AE81" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="AF81" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="AG81" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="AH81" s="2" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="82" spans="1:34" ht="16.5" customHeight="1">
-      <c r="A82" s="2">
-        <v>30</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>467</v>
@@ -6333,57 +8390,101 @@
       <c r="AH82" s="2" t="s">
         <v>505</v>
       </c>
+      <c r="AM82" t="s">
+        <v>559</v>
+      </c>
+      <c r="AU82" s="25" t="s">
+        <v>655</v>
+      </c>
     </row>
-    <row r="83" spans="1:34">
+    <row r="83" spans="1:47" ht="16.5" customHeight="1">
       <c r="A83" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H83" s="2" t="s">
         <v>467</v>
       </c>
+      <c r="V83" s="2" t="s">
+        <v>399</v>
+      </c>
       <c r="AD83" s="2" t="s">
         <v>450</v>
       </c>
       <c r="AE83" s="2" t="s">
         <v>466</v>
       </c>
+      <c r="AF83" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="AG83" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="AH83" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="AM83" t="s">
+        <v>559</v>
+      </c>
+      <c r="AU83" s="25" t="s">
+        <v>655</v>
+      </c>
     </row>
-    <row r="84" spans="1:34">
+    <row r="84" spans="1:47">
       <c r="A84" s="2">
+        <v>31</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="AD84" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="AE84" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="85" spans="1:47">
+      <c r="A85" s="2">
         <v>32</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="D85" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="85" spans="1:34">
-      <c r="A85" s="2">
+    <row r="86" spans="1:47">
+      <c r="A86" s="2">
         <v>33</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D85" s="2" t="s">
+      <c r="D86" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="86" spans="1:34">
-      <c r="A86" s="2">
+    <row r="87" spans="1:47">
+      <c r="A87" s="2">
         <v>34</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="D87" s="2" t="s">
         <v>116</v>
       </c>
     </row>
@@ -6457,8 +8558,8 @@
     <hyperlink ref="AB26" r:id="rId66"/>
     <hyperlink ref="AB28" r:id="rId67"/>
     <hyperlink ref="AB27" r:id="rId68"/>
-    <hyperlink ref="AB43" r:id="rId69" display="https://mayoverse.github.io/arsenal/reference/comparedf.html"/>
-    <hyperlink ref="AB44" r:id="rId70" display="https://mayoverse.github.io/arsenal/reference/comparedf.html"/>
+    <hyperlink ref="AB44" r:id="rId69" display="https://mayoverse.github.io/arsenal/reference/comparedf.html"/>
+    <hyperlink ref="AB45" r:id="rId70" display="https://mayoverse.github.io/arsenal/reference/comparedf.html"/>
     <hyperlink ref="AC28" r:id="rId71"/>
     <hyperlink ref="AC26" r:id="rId72"/>
     <hyperlink ref="AD27" r:id="rId73"/>
@@ -6477,8 +8578,13 @@
     <hyperlink ref="AK26" r:id="rId86"/>
     <hyperlink ref="AK28" r:id="rId87"/>
     <hyperlink ref="AK27" r:id="rId88"/>
+    <hyperlink ref="AL28" r:id="rId89"/>
+    <hyperlink ref="AN26" r:id="rId90"/>
+    <hyperlink ref="AN27" r:id="rId91"/>
+    <hyperlink ref="AN28" r:id="rId92"/>
+    <hyperlink ref="AS27" r:id="rId93"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId89"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId94"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add assertr + pointblank scripts
</commit_message>
<xml_diff>
--- a/Data quality revision R overview v01.xlsx
+++ b/Data quality revision R overview v01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="2676" tabRatio="169"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="2670" tabRatio="169"/>
   </bookViews>
   <sheets>
     <sheet name="Tools" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1716" uniqueCount="704">
   <si>
     <t>Acronym (falls vorhanden)</t>
   </si>
@@ -2252,6 +2252,15 @@
  within_n_mads - better method for dynamically creating bounds to check vector elements with based on 'robust' z-scores (using median absolute deviation)
 </t>
   </si>
+  <si>
+    <t>verify(nrow())</t>
+  </si>
+  <si>
+    <t>has_all_names - verify strict names</t>
+  </si>
+  <si>
+    <t>Custom check functions can be programmed</t>
+  </si>
 </sst>
 </file>
 
@@ -2259,7 +2268,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -2416,7 +2425,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2705,65 +2714,65 @@
   <dimension ref="A1:BA87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="AZ12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="AZ3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BA18" sqref="BA18"/>
+      <selection pane="bottomRight" activeCell="BB9" sqref="BB9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="47" style="2" customWidth="1"/>
-    <col min="5" max="5" width="43.88671875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="46.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="39.5546875" style="2" customWidth="1"/>
-    <col min="8" max="9" width="38.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="46.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="39.5703125" style="2" customWidth="1"/>
+    <col min="8" max="9" width="38.7109375" style="2" customWidth="1"/>
     <col min="10" max="10" width="42" style="2" customWidth="1"/>
-    <col min="11" max="11" width="40.44140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="32.44140625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="33.6640625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="34.33203125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="38.6640625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="32.5546875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="31.6640625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="32.6640625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="36.44140625" style="2" customWidth="1"/>
-    <col min="20" max="20" width="33.33203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="40.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="32.42578125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="33.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="34.28515625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="38.7109375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="32.5703125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="31.7109375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="32.7109375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="36.42578125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="33.28515625" style="2" customWidth="1"/>
     <col min="21" max="21" width="34" style="2" customWidth="1"/>
-    <col min="22" max="22" width="33.33203125" style="2" customWidth="1"/>
-    <col min="23" max="23" width="38.6640625" style="2" customWidth="1"/>
-    <col min="24" max="24" width="34.44140625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="33.28515625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="38.7109375" style="2" customWidth="1"/>
+    <col min="24" max="24" width="34.42578125" style="2" customWidth="1"/>
     <col min="25" max="25" width="33" style="2" customWidth="1"/>
-    <col min="26" max="26" width="33.88671875" style="2" customWidth="1"/>
-    <col min="27" max="27" width="32.88671875" style="2" customWidth="1"/>
-    <col min="28" max="28" width="36.44140625" style="2" customWidth="1"/>
-    <col min="29" max="29" width="32.6640625" style="2" customWidth="1"/>
-    <col min="30" max="30" width="32.5546875" style="2" customWidth="1"/>
-    <col min="31" max="31" width="37.33203125" style="2" customWidth="1"/>
-    <col min="32" max="32" width="38.44140625" style="2" customWidth="1"/>
-    <col min="33" max="33" width="33.109375" style="2" customWidth="1"/>
-    <col min="34" max="34" width="32.88671875" style="2" customWidth="1"/>
-    <col min="35" max="35" width="28.44140625" style="2" customWidth="1"/>
-    <col min="36" max="36" width="24.109375" style="2" customWidth="1"/>
-    <col min="37" max="37" width="22.77734375" style="2" customWidth="1"/>
+    <col min="26" max="26" width="33.85546875" style="2" customWidth="1"/>
+    <col min="27" max="27" width="32.85546875" style="2" customWidth="1"/>
+    <col min="28" max="28" width="36.42578125" style="2" customWidth="1"/>
+    <col min="29" max="29" width="32.7109375" style="2" customWidth="1"/>
+    <col min="30" max="30" width="32.5703125" style="2" customWidth="1"/>
+    <col min="31" max="31" width="37.28515625" style="2" customWidth="1"/>
+    <col min="32" max="32" width="38.42578125" style="2" customWidth="1"/>
+    <col min="33" max="33" width="33.140625" style="2" customWidth="1"/>
+    <col min="34" max="34" width="32.85546875" style="2" customWidth="1"/>
+    <col min="35" max="35" width="28.42578125" style="2" customWidth="1"/>
+    <col min="36" max="36" width="24.140625" style="2" customWidth="1"/>
+    <col min="37" max="37" width="22.7109375" style="2" customWidth="1"/>
     <col min="38" max="38" width="24" style="2" customWidth="1"/>
-    <col min="39" max="39" width="26.5546875" style="2" customWidth="1"/>
-    <col min="40" max="40" width="26.6640625" style="2" customWidth="1"/>
-    <col min="41" max="41" width="27.77734375" style="2" customWidth="1"/>
-    <col min="42" max="42" width="24.33203125" style="2" customWidth="1"/>
-    <col min="43" max="43" width="31.5546875" style="2" customWidth="1"/>
+    <col min="39" max="39" width="26.5703125" style="2" customWidth="1"/>
+    <col min="40" max="40" width="26.7109375" style="2" customWidth="1"/>
+    <col min="41" max="41" width="27.7109375" style="2" customWidth="1"/>
+    <col min="42" max="42" width="24.28515625" style="2" customWidth="1"/>
+    <col min="43" max="43" width="31.5703125" style="2" customWidth="1"/>
     <col min="44" max="44" width="26" style="2" customWidth="1"/>
-    <col min="45" max="45" width="26.109375" style="2" customWidth="1"/>
-    <col min="46" max="46" width="25.6640625" style="2" customWidth="1"/>
-    <col min="47" max="47" width="29.44140625" style="2" customWidth="1"/>
-    <col min="48" max="48" width="29.5546875" style="2" customWidth="1"/>
-    <col min="49" max="49" width="26.88671875" style="2" customWidth="1"/>
-    <col min="50" max="50" width="25.6640625" style="2" customWidth="1"/>
-    <col min="51" max="52" width="28.33203125" style="2" customWidth="1"/>
-    <col min="53" max="53" width="25.21875" style="2" customWidth="1"/>
+    <col min="45" max="45" width="26.140625" style="2" customWidth="1"/>
+    <col min="46" max="46" width="25.7109375" style="2" customWidth="1"/>
+    <col min="47" max="47" width="29.42578125" style="2" customWidth="1"/>
+    <col min="48" max="48" width="29.5703125" style="2" customWidth="1"/>
+    <col min="49" max="49" width="26.85546875" style="2" customWidth="1"/>
+    <col min="50" max="50" width="25.7109375" style="2" customWidth="1"/>
+    <col min="51" max="52" width="28.28515625" style="2" customWidth="1"/>
+    <col min="53" max="53" width="25.28515625" style="2" customWidth="1"/>
     <col min="54" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
@@ -2925,7 +2934,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="2" spans="2:53" ht="28.8">
+    <row r="2" spans="2:53" ht="30">
       <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
@@ -3712,7 +3721,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:53" ht="28.8">
+    <row r="7" spans="2:53" ht="45">
       <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
@@ -3867,7 +3876,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:53" ht="28.8">
+    <row r="8" spans="2:53" ht="30">
       <c r="B8" s="2" t="s">
         <v>40</v>
       </c>
@@ -4174,7 +4183,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="10" spans="2:53">
+    <row r="10" spans="2:53" ht="30">
       <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
@@ -4332,7 +4341,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:53" ht="28.8">
+    <row r="11" spans="2:53" ht="30">
       <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
@@ -4490,7 +4499,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:53" ht="115.2">
+    <row r="12" spans="2:53" ht="135">
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
@@ -4754,9 +4763,11 @@
       <c r="AU13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="BA13"/>
+      <c r="BA13" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="14" spans="2:53" ht="28.8">
+    <row r="14" spans="2:53" ht="30">
       <c r="B14" s="2" t="s">
         <v>45</v>
       </c>
@@ -4865,8 +4876,11 @@
       <c r="AU14" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="BA14" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="15" spans="2:53" ht="28.8">
+    <row r="15" spans="2:53" ht="30">
       <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
@@ -4974,6 +4988,9 @@
       </c>
       <c r="AU15" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="BA15" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="2:53" ht="27.6" customHeight="1">
@@ -5088,8 +5105,11 @@
       <c r="AU16" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="BA16" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="17" spans="2:53" ht="151.19999999999999" customHeight="1">
+    <row r="17" spans="2:53" ht="151.15" customHeight="1">
       <c r="B17" s="2" t="s">
         <v>44</v>
       </c>
@@ -5196,7 +5216,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="18" spans="2:53" ht="28.8">
+    <row r="18" spans="2:53" ht="30">
       <c r="B18" s="2" t="s">
         <v>27</v>
       </c>
@@ -5339,7 +5359,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:53" ht="28.8">
+    <row r="19" spans="2:53" ht="45">
       <c r="B19" s="2" t="s">
         <v>28</v>
       </c>
@@ -5482,7 +5502,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:53" ht="28.8">
+    <row r="20" spans="2:53" ht="30">
       <c r="B20" s="2" t="s">
         <v>29</v>
       </c>
@@ -5625,7 +5645,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:53" ht="28.8">
+    <row r="21" spans="2:53" ht="30">
       <c r="B21" s="2" t="s">
         <v>30</v>
       </c>
@@ -5765,7 +5785,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="22" spans="2:53" ht="28.8">
+    <row r="22" spans="2:53" ht="30">
       <c r="B22" s="2" t="s">
         <v>35</v>
       </c>
@@ -5914,7 +5934,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:53" ht="28.8">
+    <row r="23" spans="2:53" ht="30">
       <c r="B23" s="2" t="s">
         <v>37</v>
       </c>
@@ -6057,7 +6077,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:53" ht="28.8">
+    <row r="24" spans="2:53" ht="30">
       <c r="B24" s="2" t="s">
         <v>39</v>
       </c>
@@ -6318,7 +6338,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="26" spans="2:53" ht="43.2">
+    <row r="26" spans="2:53" ht="45">
       <c r="B26" s="2" t="s">
         <v>137</v>
       </c>
@@ -6434,7 +6454,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="27" spans="2:53" ht="43.2">
+    <row r="27" spans="2:53" ht="60">
       <c r="B27" s="2" t="s">
         <v>3</v>
       </c>
@@ -6547,7 +6567,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="28" spans="2:53" ht="28.8">
+    <row r="28" spans="2:53" ht="45">
       <c r="B28" s="2" t="s">
         <v>32</v>
       </c>
@@ -6696,7 +6716,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="29" spans="2:53" ht="172.8">
+    <row r="29" spans="2:53" ht="195">
       <c r="D29" s="3" t="s">
         <v>140</v>
       </c>
@@ -6727,13 +6747,13 @@
         <v>675</v>
       </c>
     </row>
-    <row r="30" spans="2:53" ht="28.8">
+    <row r="30" spans="2:53" ht="30">
       <c r="D30" s="3"/>
       <c r="AO30" s="2" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="31" spans="2:53" ht="28.8">
+    <row r="31" spans="2:53" ht="30">
       <c r="B31" s="2" t="s">
         <v>33</v>
       </c>
@@ -7457,7 +7477,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:53" ht="86.4">
+    <row r="38" spans="1:53" ht="105">
       <c r="B38" s="2" t="s">
         <v>233</v>
       </c>
@@ -7564,8 +7584,11 @@
       <c r="AZ38" s="2" t="s">
         <v>686</v>
       </c>
+      <c r="BA38" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
-    <row r="39" spans="1:53" ht="57.6">
+    <row r="39" spans="1:53" ht="60">
       <c r="B39" s="2" t="s">
         <v>561</v>
       </c>
@@ -7646,6 +7669,9 @@
       <c r="AL44" s="2" t="s">
         <v>544</v>
       </c>
+      <c r="BA44" s="2" t="s">
+        <v>701</v>
+      </c>
     </row>
     <row r="45" spans="1:53">
       <c r="A45" s="2">
@@ -7807,7 +7833,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="50" spans="1:53">
+    <row r="50" spans="1:53" ht="30">
       <c r="A50" s="2">
         <v>7</v>
       </c>
@@ -7822,6 +7848,9 @@
       </c>
       <c r="J50" s="2" t="s">
         <v>161</v>
+      </c>
+      <c r="BA50" s="2" t="s">
+        <v>702</v>
       </c>
     </row>
     <row r="51" spans="1:53">
@@ -7870,7 +7899,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="53" spans="1:53" ht="28.8">
+    <row r="53" spans="1:53" ht="30">
       <c r="E53" s="2" t="s">
         <v>395</v>
       </c>
@@ -7893,7 +7922,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="54" spans="1:53">
+    <row r="54" spans="1:53" ht="30">
       <c r="E54" s="2" t="s">
         <v>129</v>
       </c>
@@ -7920,7 +7949,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="1:53" ht="28.8">
+    <row r="57" spans="1:53" ht="30">
       <c r="A57" s="2">
         <v>9</v>
       </c>
@@ -8039,7 +8068,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:53" ht="28.8">
+    <row r="61" spans="1:53" ht="30">
       <c r="A61" s="2">
         <v>13</v>
       </c>
@@ -8061,7 +8090,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="64" spans="1:53" ht="28.8">
+    <row r="64" spans="1:53" ht="30">
       <c r="A64" s="2">
         <v>14</v>
       </c>
@@ -8097,11 +8126,8 @@
       <c r="AS65" s="2" t="s">
         <v>632</v>
       </c>
-      <c r="BA65" s="2" t="s">
-        <v>696</v>
-      </c>
     </row>
-    <row r="66" spans="1:53" ht="28.8">
+    <row r="66" spans="1:53" ht="30">
       <c r="A66" s="2">
         <v>16</v>
       </c>
@@ -8118,7 +8144,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="67" spans="1:53" ht="28.8">
+    <row r="67" spans="1:53" ht="30">
       <c r="A67" s="2">
         <v>17</v>
       </c>
@@ -8127,6 +8153,9 @@
       </c>
       <c r="D67" s="2" t="s">
         <v>98</v>
+      </c>
+      <c r="BA67" s="2" t="s">
+        <v>697</v>
       </c>
     </row>
     <row r="68" spans="1:53">
@@ -8140,7 +8169,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="69" spans="1:53" ht="28.8">
+    <row r="69" spans="1:53" ht="30">
       <c r="A69" s="2">
         <v>19</v>
       </c>
@@ -8173,11 +8202,8 @@
       <c r="J70" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="BA70" s="2" t="s">
-        <v>696</v>
-      </c>
     </row>
-    <row r="71" spans="1:53" ht="28.8">
+    <row r="71" spans="1:53" ht="30">
       <c r="A71" s="2">
         <v>21</v>
       </c>
@@ -8278,7 +8304,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="79" spans="1:53" ht="28.8">
+    <row r="79" spans="1:53" ht="30">
       <c r="A79" s="2">
         <v>26</v>
       </c>
@@ -8477,7 +8503,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="87" spans="1:47">
+    <row r="87" spans="1:47" ht="30">
       <c r="A87" s="2">
         <v>34</v>
       </c>

</xml_diff>